<commit_message>
Updates to docs, saved Azure templates
</commit_message>
<xml_diff>
--- a/Mifos-io-environment-details.xlsx
+++ b/Mifos-io-environment-details.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sconrad/DIAL/t4d-product-backlog/fineract/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C5267FE-A005-5749-BD7D-7F7C18469DA3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E818BD7-798E-E747-B9A5-4F01232955B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="27860" windowHeight="17580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1220" yWindow="840" windowWidth="27860" windowHeight="17580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Environment details" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,20 @@
     <sheet name="Fineract REST API" sheetId="4" r:id="rId4"/>
     <sheet name="Types" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="292">
   <si>
     <t>URL</t>
   </si>
@@ -856,29 +864,74 @@
     <t>fincn.mifos.io</t>
   </si>
   <si>
-    <t>https://fineract.mifos.io:9002/?baseApiUrl=https://fineract.mifos.io:8443&amp;tenantIdentifier=tn01</t>
-  </si>
-  <si>
-    <t>https://fineract.mifos.io:9002/?baseApiUrl=https://fineract.mifos.io:8443&amp;tenantIdentifier=tn02</t>
-  </si>
-  <si>
-    <t>http://fincn.mifos.io:9002/?baseApiUrl=https://fincn.mifos.io:8443&amp;tenantIdentifier=tn03</t>
-  </si>
-  <si>
-    <t>http://fincn.mifos.io:9002/?baseApiUrl=https://fincn.mifos.io:8443&amp;tenantIdentifier=tn04</t>
-  </si>
-  <si>
-    <t>https://fineract.mifos.io:8443/fineract-provider/api/v1</t>
-  </si>
-  <si>
-    <t>https://fincn.mifos.io:8443/fineract-provider/api/v1</t>
+    <t>http://paymenthub.mifos.io/channel</t>
+  </si>
+  <si>
+    <t>http://paymenthubcn.mifos.io/channel</t>
+  </si>
+  <si>
+    <t>http://buffalo.mifos.io:9002/?baseApiUrl=https://buffalo.mifos.io:8443&amp;tenantIdentifier=tn01</t>
+  </si>
+  <si>
+    <t>https://buffalo.mifos.io:8443/fineract-provider/api/v1</t>
+  </si>
+  <si>
+    <t>https://lion.mifos.io:8443/fineract-provider/api/v1</t>
+  </si>
+  <si>
+    <t>http://lion.mifos.io:9002/?baseApiUrl=https://lion.mifos.io:8443&amp;tenantIdentifier=tn02</t>
+  </si>
+  <si>
+    <t>https://rhino.mifos.io:8443/fineract-provider/api/v1</t>
+  </si>
+  <si>
+    <t>http://rhino.mifos.io:9002/?baseApiUrl=https://rhino.mifos.io:8443&amp;tenantIdentifier=tn03</t>
+  </si>
+  <si>
+    <t>http://elephant.mifos.io:9002/?baseApiUrl=https://elephant.mifos.io:8443&amp;tenantIdentifier=tn04</t>
+  </si>
+  <si>
+    <t>https://elephant.mifos.io:8443/fineract-provider/api/v1</t>
+  </si>
+  <si>
+    <t>api.lion.mifos.io</t>
+  </si>
+  <si>
+    <t>https://api.lion.mifos.io:8243/ais/v1</t>
+  </si>
+  <si>
+    <t>https://api.lion.mifos.io:8243/pis/v1</t>
+  </si>
+  <si>
+    <t>https://api.lion.mifos.io:8243/store</t>
+  </si>
+  <si>
+    <t>https://lion.mifos.io/netbank</t>
+  </si>
+  <si>
+    <t>api.elephant.mifos.io</t>
+  </si>
+  <si>
+    <t>https://api.elephant.mifos.io:8243/ais/v1</t>
+  </si>
+  <si>
+    <t>https://api.elephant.mifos.io:8243/pis/v1</t>
+  </si>
+  <si>
+    <t>https://api.elephant.mifos.io:8243/store</t>
+  </si>
+  <si>
+    <t>https://elephant.mifos.io/netbank</t>
+  </si>
+  <si>
+    <t>http://acefintech.mifos.io</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -984,6 +1037,13 @@
       <sz val="10"/>
       <color theme="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF1155CC"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1194,7 +1254,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1300,16 +1360,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1321,7 +1381,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1330,14 +1395,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1660,10 +1721,10 @@
   <dimension ref="A1:Y1010"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B24" sqref="B24:E27"/>
+      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1676,14 +1737,14 @@
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="76"/>
-      <c r="D1" s="77" t="s">
+      <c r="C1" s="77"/>
+      <c r="D1" s="79" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="76"/>
+      <c r="E1" s="77"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1709,10 +1770,10 @@
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1">
@@ -1738,14 +1799,14 @@
       <c r="A4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="76" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="79" t="s">
+      <c r="C4" s="77"/>
+      <c r="D4" s="76" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="76"/>
+      <c r="E4" s="77"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
@@ -1821,10 +1882,12 @@
       <c r="A9" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="80"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="76"/>
-      <c r="E9" s="76"/>
+      <c r="B9" s="96" t="s">
+        <v>291</v>
+      </c>
+      <c r="C9" s="77"/>
+      <c r="D9" s="77"/>
+      <c r="E9" s="77"/>
       <c r="F9" s="6"/>
       <c r="G9" s="39"/>
     </row>
@@ -1833,9 +1896,13 @@
         <v>84</v>
       </c>
       <c r="B10" s="37"/>
-      <c r="C10" s="37"/>
+      <c r="C10" s="13" t="s">
+        <v>281</v>
+      </c>
       <c r="D10" s="37"/>
-      <c r="E10" s="37"/>
+      <c r="E10" s="95" t="s">
+        <v>286</v>
+      </c>
       <c r="F10" s="6"/>
       <c r="G10" s="39"/>
     </row>
@@ -1844,9 +1911,13 @@
         <v>88</v>
       </c>
       <c r="B11" s="37"/>
-      <c r="C11" s="37"/>
+      <c r="C11" s="75" t="s">
+        <v>282</v>
+      </c>
       <c r="D11" s="37"/>
-      <c r="E11" s="37"/>
+      <c r="E11" s="75" t="s">
+        <v>287</v>
+      </c>
       <c r="F11" s="6"/>
       <c r="G11" s="39"/>
     </row>
@@ -1855,9 +1926,13 @@
         <v>97</v>
       </c>
       <c r="B12" s="37"/>
-      <c r="C12" s="37"/>
+      <c r="C12" s="75" t="s">
+        <v>283</v>
+      </c>
       <c r="D12" s="37"/>
-      <c r="E12" s="37"/>
+      <c r="E12" s="75" t="s">
+        <v>288</v>
+      </c>
       <c r="F12" s="6"/>
       <c r="G12" s="39"/>
     </row>
@@ -1866,9 +1941,13 @@
         <v>124</v>
       </c>
       <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
+      <c r="C13" s="75" t="s">
+        <v>284</v>
+      </c>
       <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
+      <c r="E13" s="75" t="s">
+        <v>289</v>
+      </c>
       <c r="F13" s="6"/>
       <c r="G13" s="39"/>
     </row>
@@ -1877,9 +1956,13 @@
         <v>161</v>
       </c>
       <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
+      <c r="C14" s="75" t="s">
+        <v>285</v>
+      </c>
       <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
+      <c r="E14" s="75" t="s">
+        <v>290</v>
+      </c>
       <c r="F14" s="6"/>
       <c r="G14" s="39"/>
     </row>
@@ -1917,17 +2000,17 @@
       <c r="A17" s="31" t="s">
         <v>215</v>
       </c>
-      <c r="B17" s="95" t="s">
-        <v>271</v>
-      </c>
-      <c r="C17" s="95" t="s">
-        <v>272</v>
-      </c>
-      <c r="D17" s="95" t="s">
+      <c r="B17" s="75" t="s">
         <v>273</v>
       </c>
-      <c r="E17" s="95" t="s">
-        <v>274</v>
+      <c r="C17" s="75" t="s">
+        <v>276</v>
+      </c>
+      <c r="D17" s="75" t="s">
+        <v>278</v>
+      </c>
+      <c r="E17" s="75" t="s">
+        <v>279</v>
       </c>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
@@ -1955,17 +2038,17 @@
       <c r="A19" s="68" t="s">
         <v>249</v>
       </c>
-      <c r="B19" s="95" t="s">
+      <c r="B19" s="75" t="s">
+        <v>274</v>
+      </c>
+      <c r="C19" s="75" t="s">
         <v>275</v>
       </c>
-      <c r="C19" s="95" t="s">
-        <v>275</v>
-      </c>
-      <c r="D19" s="95" t="s">
-        <v>276</v>
-      </c>
-      <c r="E19" s="95" t="s">
-        <v>276</v>
+      <c r="D19" s="75" t="s">
+        <v>277</v>
+      </c>
+      <c r="E19" s="75" t="s">
+        <v>280</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="70"/>
@@ -2086,10 +2169,18 @@
       <c r="A24" s="9" t="s">
         <v>265</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="13"/>
-      <c r="E24" s="13"/>
+      <c r="B24" s="75" t="s">
+        <v>271</v>
+      </c>
+      <c r="C24" s="75" t="s">
+        <v>271</v>
+      </c>
+      <c r="D24" s="75" t="s">
+        <v>272</v>
+      </c>
+      <c r="E24" s="13" t="s">
+        <v>272</v>
+      </c>
       <c r="F24" s="6"/>
     </row>
     <row r="25" spans="1:25" ht="15.75" customHeight="1">
@@ -2106,19 +2197,19 @@
       <c r="A26" s="9" t="s">
         <v>267</v>
       </c>
-      <c r="B26" s="79"/>
-      <c r="C26" s="76"/>
-      <c r="D26" s="76"/>
-      <c r="E26" s="76"/>
+      <c r="B26" s="76"/>
+      <c r="C26" s="77"/>
+      <c r="D26" s="77"/>
+      <c r="E26" s="77"/>
       <c r="F26" s="6"/>
     </row>
     <row r="27" spans="1:25" ht="15.75" customHeight="1">
       <c r="A27" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="B27" s="95"/>
+      <c r="B27" s="75"/>
       <c r="C27" s="21"/>
-      <c r="D27" s="95"/>
+      <c r="D27" s="75"/>
       <c r="E27" s="13"/>
       <c r="F27" s="6"/>
     </row>
@@ -6208,6 +6299,18 @@
     <hyperlink ref="C19" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
     <hyperlink ref="D19" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
     <hyperlink ref="E19" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B24" r:id="rId13" xr:uid="{9D45292F-4DF7-FB46-A4BB-FE81BB0CAFD7}"/>
+    <hyperlink ref="C24" r:id="rId14" xr:uid="{7B808EA3-3AE1-3943-8E7A-54B1456282A4}"/>
+    <hyperlink ref="D24" r:id="rId15" xr:uid="{4DEB1400-E116-8A47-8E39-BA0366DC40E1}"/>
+    <hyperlink ref="C11" r:id="rId16" xr:uid="{FEBE3A66-3830-9040-8A39-8224B5F40D3C}"/>
+    <hyperlink ref="C12" r:id="rId17" xr:uid="{2E96C83A-AC7A-3145-99A7-8C46E9E18660}"/>
+    <hyperlink ref="C13" r:id="rId18" xr:uid="{484A1410-AE50-F046-A9F6-25DDF752262B}"/>
+    <hyperlink ref="C14" r:id="rId19" xr:uid="{8FAA37D5-02E1-2042-A463-C14CC8D5E9E5}"/>
+    <hyperlink ref="E11" r:id="rId20" xr:uid="{2261E2D5-70E3-994D-BFD7-97C517740E9A}"/>
+    <hyperlink ref="E12" r:id="rId21" xr:uid="{E051FC20-56A9-794C-B194-55B421D51523}"/>
+    <hyperlink ref="E13" r:id="rId22" xr:uid="{0CDAC340-0A45-8F41-8CF9-D804202312D5}"/>
+    <hyperlink ref="E14" r:id="rId23" xr:uid="{2B07D10D-DE71-3F4B-8CD5-0423AC1A4ACE}"/>
+    <hyperlink ref="B9" r:id="rId24" xr:uid="{F0D4CA2C-A633-7647-BE50-42059087D399}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6845,8 +6948,8 @@
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
       <c r="K7" s="84"/>
-      <c r="L7" s="76"/>
-      <c r="M7" s="76"/>
+      <c r="L7" s="77"/>
+      <c r="M7" s="77"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1">
       <c r="B8" s="9"/>
@@ -6869,8 +6972,8 @@
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
       <c r="K10" s="84"/>
-      <c r="L10" s="76"/>
-      <c r="M10" s="76"/>
+      <c r="L10" s="77"/>
+      <c r="M10" s="77"/>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
@@ -6902,8 +7005,8 @@
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
       <c r="K13" s="84"/>
-      <c r="L13" s="76"/>
-      <c r="M13" s="76"/>
+      <c r="L13" s="77"/>
+      <c r="M13" s="77"/>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
@@ -6973,8 +7076,8 @@
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
       <c r="K21" s="84"/>
-      <c r="L21" s="76"/>
-      <c r="M21" s="76"/>
+      <c r="L21" s="77"/>
+      <c r="M21" s="77"/>
     </row>
     <row r="22" spans="2:17" ht="15.75" customHeight="1">
       <c r="B22" s="9"/>
@@ -6993,8 +7096,8 @@
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
       <c r="K23" s="84"/>
-      <c r="L23" s="76"/>
-      <c r="M23" s="76"/>
+      <c r="L23" s="77"/>
+      <c r="M23" s="77"/>
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
@@ -7140,8 +7243,8 @@
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
       <c r="K36" s="84"/>
-      <c r="L36" s="76"/>
-      <c r="M36" s="76"/>
+      <c r="L36" s="77"/>
+      <c r="M36" s="77"/>
     </row>
     <row r="37" spans="2:17" ht="15.75" customHeight="1">
       <c r="B37" s="9"/>
@@ -7162,8 +7265,8 @@
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
       <c r="K38" s="84"/>
-      <c r="L38" s="76"/>
-      <c r="M38" s="76"/>
+      <c r="L38" s="77"/>
+      <c r="M38" s="77"/>
       <c r="N38" s="9"/>
       <c r="O38" s="9"/>
       <c r="P38" s="9"/>
@@ -7313,24 +7416,24 @@
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
       <c r="K51" s="84"/>
-      <c r="L51" s="76"/>
-      <c r="M51" s="76"/>
+      <c r="L51" s="77"/>
+      <c r="M51" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="K51:M51"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K13:M13"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="K23:M23"/>
+    <mergeCell ref="K36:M36"/>
+    <mergeCell ref="K38:M38"/>
     <mergeCell ref="K7:M7"/>
     <mergeCell ref="K21:M21"/>
     <mergeCell ref="K5:M5"/>
     <mergeCell ref="N1:Q1"/>
     <mergeCell ref="K1:M1"/>
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="E1:G1"/>
-    <mergeCell ref="K23:M23"/>
-    <mergeCell ref="K36:M36"/>
-    <mergeCell ref="K38:M38"/>
-    <mergeCell ref="K51:M51"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="K13:M13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7565,11 +7668,11 @@
       <c r="H6" s="27"/>
       <c r="I6" s="27"/>
       <c r="J6" s="27"/>
-      <c r="K6" s="86" t="s">
+      <c r="K6" s="94" t="s">
         <v>106</v>
       </c>
-      <c r="L6" s="87"/>
-      <c r="M6" s="87"/>
+      <c r="L6" s="90"/>
+      <c r="M6" s="90"/>
       <c r="N6" s="18" t="s">
         <v>107</v>
       </c>
@@ -7646,11 +7749,11 @@
       <c r="H9" s="26"/>
       <c r="I9" s="27"/>
       <c r="J9" s="27"/>
-      <c r="K9" s="86" t="s">
+      <c r="K9" s="94" t="s">
         <v>106</v>
       </c>
-      <c r="L9" s="87"/>
-      <c r="M9" s="87"/>
+      <c r="L9" s="90"/>
+      <c r="M9" s="90"/>
       <c r="N9" s="26"/>
       <c r="O9" s="27"/>
       <c r="P9" s="27"/>
@@ -7727,11 +7830,11 @@
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
       <c r="J12" s="27"/>
-      <c r="K12" s="86" t="s">
+      <c r="K12" s="94" t="s">
         <v>106</v>
       </c>
-      <c r="L12" s="87"/>
-      <c r="M12" s="87"/>
+      <c r="L12" s="90"/>
+      <c r="M12" s="90"/>
       <c r="N12" s="18"/>
       <c r="O12" s="20"/>
       <c r="P12" s="20"/>
@@ -7794,11 +7897,11 @@
       <c r="H15" s="26"/>
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
-      <c r="K15" s="86" t="s">
+      <c r="K15" s="94" t="s">
         <v>106</v>
       </c>
-      <c r="L15" s="87"/>
-      <c r="M15" s="87"/>
+      <c r="L15" s="90"/>
+      <c r="M15" s="90"/>
       <c r="N15" s="18" t="s">
         <v>122</v>
       </c>
@@ -7996,11 +8099,11 @@
       <c r="H23" s="26"/>
       <c r="I23" s="27"/>
       <c r="J23" s="27"/>
-      <c r="K23" s="86" t="s">
+      <c r="K23" s="94" t="s">
         <v>106</v>
       </c>
-      <c r="L23" s="87"/>
-      <c r="M23" s="88"/>
+      <c r="L23" s="90"/>
+      <c r="M23" s="91"/>
       <c r="N23" s="26"/>
       <c r="O23" s="27"/>
       <c r="P23" s="27"/>
@@ -8041,11 +8144,11 @@
       <c r="E25" s="18"/>
       <c r="F25" s="20"/>
       <c r="G25" s="22"/>
-      <c r="K25" s="86" t="s">
+      <c r="K25" s="94" t="s">
         <v>106</v>
       </c>
-      <c r="L25" s="87"/>
-      <c r="M25" s="88"/>
+      <c r="L25" s="90"/>
+      <c r="M25" s="91"/>
       <c r="N25" s="18" t="s">
         <v>122</v>
       </c>
@@ -8370,11 +8473,11 @@
       <c r="H38" s="26"/>
       <c r="I38" s="27"/>
       <c r="J38" s="27"/>
-      <c r="K38" s="89" t="s">
+      <c r="K38" s="92" t="s">
         <v>106</v>
       </c>
-      <c r="L38" s="76"/>
-      <c r="M38" s="90"/>
+      <c r="L38" s="77"/>
+      <c r="M38" s="93"/>
       <c r="N38" s="24"/>
       <c r="Q38" s="25"/>
       <c r="S38" s="51"/>
@@ -8424,11 +8527,11 @@
       <c r="J40" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="K40" s="86" t="s">
+      <c r="K40" s="94" t="s">
         <v>106</v>
       </c>
-      <c r="L40" s="87"/>
-      <c r="M40" s="88"/>
+      <c r="L40" s="90"/>
+      <c r="M40" s="91"/>
       <c r="N40" s="18" t="s">
         <v>122</v>
       </c>
@@ -8781,11 +8884,11 @@
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
       <c r="H53" s="24"/>
-      <c r="K53" s="89" t="s">
+      <c r="K53" s="92" t="s">
         <v>106</v>
       </c>
-      <c r="L53" s="76"/>
-      <c r="M53" s="90"/>
+      <c r="L53" s="77"/>
+      <c r="M53" s="93"/>
       <c r="N53" s="26"/>
       <c r="O53" s="27"/>
       <c r="P53" s="27"/>
@@ -8803,9 +8906,9 @@
       <c r="H54" s="30"/>
       <c r="I54" s="35"/>
       <c r="J54" s="35"/>
-      <c r="K54" s="91"/>
-      <c r="L54" s="92"/>
-      <c r="M54" s="93"/>
+      <c r="K54" s="86"/>
+      <c r="L54" s="87"/>
+      <c r="M54" s="88"/>
       <c r="N54" s="30"/>
       <c r="O54" s="35"/>
       <c r="P54" s="35"/>
@@ -8837,11 +8940,11 @@
       <c r="S57" s="51"/>
     </row>
     <row r="58" spans="1:19" ht="15.75" customHeight="1">
-      <c r="K58" s="94" t="s">
+      <c r="K58" s="89" t="s">
         <v>106</v>
       </c>
-      <c r="L58" s="87"/>
-      <c r="M58" s="88"/>
+      <c r="L58" s="90"/>
+      <c r="M58" s="91"/>
       <c r="S58" s="53"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" customHeight="1">
@@ -8880,6 +8983,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K23:M23"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="K54:M54"/>
@@ -8888,11 +8996,6 @@
     <mergeCell ref="K40:M40"/>
     <mergeCell ref="K12:M12"/>
     <mergeCell ref="K15:M15"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K23:M23"/>
     <mergeCell ref="K25:M25"/>
     <mergeCell ref="K38:M38"/>
   </mergeCells>

</xml_diff>

<commit_message>
Updates for openbanking adapter
</commit_message>
<xml_diff>
--- a/Mifos-io-environment-details.xlsx
+++ b/Mifos-io-environment-details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sconrad/DIAL/t4d-product-backlog/fineract/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sconrad/DIAL/mifos/mifos-io-configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E818BD7-798E-E747-B9A5-4F01232955B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBFAD75-356E-5749-A435-CA5EA28AEB4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1220" yWindow="840" windowWidth="27860" windowHeight="17580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="301">
   <si>
     <t>URL</t>
   </si>
@@ -925,6 +925,33 @@
   </si>
   <si>
     <t>http://acefintech.mifos.io</t>
+  </si>
+  <si>
+    <t>83c4ed1c074b484e85cc79</t>
+  </si>
+  <si>
+    <t>client id</t>
+  </si>
+  <si>
+    <t>31d77b06141c11e9ab14d6</t>
+  </si>
+  <si>
+    <t>9062b90de19b43989005d9</t>
+  </si>
+  <si>
+    <t>a6b6c10b2aaa4778ac2fc9</t>
+  </si>
+  <si>
+    <t>https://lion.mifos.io:8443/fineract-provider/api/v1/interoperation</t>
+  </si>
+  <si>
+    <t>https://buffalo.mifos.io:8443/fineract-provider/api/v1/interoperation</t>
+  </si>
+  <si>
+    <t>https://rhino.mifos.io:8443/fineract-provider/api/v1/interoperation</t>
+  </si>
+  <si>
+    <t>https://elephant.mifos.io:8443/fineract-provider/api/v1/interoperation</t>
   </si>
 </sst>
 </file>
@@ -1254,7 +1281,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1363,6 +1390,11 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1381,6 +1413,11 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1389,17 +1426,10 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1718,13 +1748,13 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Y1010"/>
+  <dimension ref="A1:Y1011"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1737,14 +1767,14 @@
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="78" t="s">
+      <c r="B1" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="77"/>
-      <c r="D1" s="79" t="s">
+      <c r="C1" s="81"/>
+      <c r="D1" s="84" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="77"/>
+      <c r="E1" s="81"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1770,10 +1800,10 @@
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="77"/>
-      <c r="E2" s="77"/>
+      <c r="B2" s="85"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
       <c r="F2" s="6"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1">
@@ -1799,14 +1829,14 @@
       <c r="A4" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="76" t="s">
+      <c r="B4" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="77"/>
-      <c r="D4" s="76" t="s">
+      <c r="C4" s="81"/>
+      <c r="D4" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="E4" s="77"/>
+      <c r="E4" s="81"/>
       <c r="F4" s="6"/>
       <c r="G4" s="6"/>
     </row>
@@ -1882,12 +1912,12 @@
       <c r="A9" s="42" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="96" t="s">
+      <c r="B9" s="82" t="s">
         <v>291</v>
       </c>
-      <c r="C9" s="77"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="77"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
       <c r="F9" s="6"/>
       <c r="G9" s="39"/>
     </row>
@@ -1900,7 +1930,7 @@
         <v>281</v>
       </c>
       <c r="D10" s="37"/>
-      <c r="E10" s="95" t="s">
+      <c r="E10" s="78" t="s">
         <v>286</v>
       </c>
       <c r="F10" s="6"/>
@@ -2038,16 +2068,16 @@
       <c r="A19" s="68" t="s">
         <v>249</v>
       </c>
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="79" t="s">
         <v>274</v>
       </c>
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="79" t="s">
         <v>275</v>
       </c>
-      <c r="D19" s="75" t="s">
+      <c r="D19" s="79" t="s">
         <v>277</v>
       </c>
-      <c r="E19" s="75" t="s">
+      <c r="E19" s="79" t="s">
         <v>280</v>
       </c>
       <c r="F19" s="6"/>
@@ -2076,10 +2106,10 @@
       <c r="A21" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="B21" s="11" t="s">
+      <c r="B21" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="C21" s="9" t="s">
         <v>258</v>
       </c>
       <c r="D21" s="6" t="s">
@@ -2132,17 +2162,17 @@
       <c r="A23" s="72" t="s">
         <v>264</v>
       </c>
-      <c r="B23" s="11">
-        <v>12345</v>
-      </c>
-      <c r="C23" s="11">
-        <v>54321</v>
-      </c>
-      <c r="D23" s="6">
-        <v>23456</v>
-      </c>
-      <c r="E23" s="6">
-        <v>65432</v>
+      <c r="B23" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>296</v>
       </c>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
@@ -2165,62 +2195,98 @@
       <c r="X23" s="6"/>
       <c r="Y23" s="6"/>
     </row>
-    <row r="24" spans="1:25" ht="15.75" customHeight="1">
+    <row r="24" spans="1:25" s="77" customFormat="1" ht="15.75" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>265</v>
-      </c>
-      <c r="B24" s="75" t="s">
-        <v>271</v>
-      </c>
-      <c r="C24" s="75" t="s">
-        <v>271</v>
-      </c>
-      <c r="D24" s="75" t="s">
-        <v>272</v>
-      </c>
-      <c r="E24" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="F24" s="6"/>
+        <v>293</v>
+      </c>
+      <c r="B24" s="9">
+        <v>1</v>
+      </c>
+      <c r="C24" s="9">
+        <v>1</v>
+      </c>
+      <c r="D24" s="76">
+        <v>1</v>
+      </c>
+      <c r="E24" s="76">
+        <v>1</v>
+      </c>
+      <c r="F24" s="76"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="76"/>
+      <c r="I24" s="76"/>
+      <c r="J24" s="76"/>
+      <c r="K24" s="76"/>
+      <c r="L24" s="76"/>
+      <c r="M24" s="76"/>
+      <c r="N24" s="76"/>
+      <c r="O24" s="76"/>
+      <c r="P24" s="76"/>
+      <c r="Q24" s="76"/>
+      <c r="R24" s="76"/>
+      <c r="S24" s="76"/>
+      <c r="T24" s="76"/>
+      <c r="U24" s="76"/>
+      <c r="V24" s="76"/>
+      <c r="W24" s="76"/>
+      <c r="X24" s="76"/>
+      <c r="Y24" s="76"/>
     </row>
     <row r="25" spans="1:25" ht="15.75" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>266</v>
-      </c>
-      <c r="B25" s="73"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="70"/>
+        <v>265</v>
+      </c>
+      <c r="B25" s="75" t="s">
+        <v>271</v>
+      </c>
+      <c r="C25" s="75" t="s">
+        <v>271</v>
+      </c>
+      <c r="D25" s="75" t="s">
+        <v>272</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>272</v>
+      </c>
       <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:25" ht="15.75" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="B26" s="76"/>
-      <c r="C26" s="77"/>
-      <c r="D26" s="77"/>
-      <c r="E26" s="77"/>
+        <v>266</v>
+      </c>
+      <c r="B26" s="73"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="70"/>
+      <c r="E26" s="70"/>
       <c r="F26" s="6"/>
     </row>
     <row r="27" spans="1:25" ht="15.75" customHeight="1">
       <c r="A27" s="9" t="s">
+        <v>267</v>
+      </c>
+      <c r="B27" s="80"/>
+      <c r="C27" s="81"/>
+      <c r="D27" s="81"/>
+      <c r="E27" s="81"/>
+      <c r="F27" s="6"/>
+    </row>
+    <row r="28" spans="1:25" ht="15.75" customHeight="1">
+      <c r="A28" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="B27" s="75"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="13"/>
-      <c r="F27" s="6"/>
-    </row>
-    <row r="28" spans="1:25" ht="15.75" customHeight="1">
-      <c r="A28" s="9"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
+      <c r="B28" s="79" t="s">
+        <v>298</v>
+      </c>
+      <c r="C28" s="79" t="s">
+        <v>297</v>
+      </c>
+      <c r="D28" s="79" t="s">
+        <v>299</v>
+      </c>
+      <c r="E28" s="79" t="s">
+        <v>300</v>
+      </c>
+      <c r="F28" s="6"/>
     </row>
     <row r="29" spans="1:25" ht="15.75" customHeight="1">
       <c r="A29" s="9"/>
@@ -2448,8 +2514,13 @@
       <c r="G53" s="9"/>
     </row>
     <row r="54" spans="1:7" ht="15.75" customHeight="1">
-      <c r="B54" s="74"/>
-      <c r="C54" s="74"/>
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="9"/>
+      <c r="F54" s="9"/>
+      <c r="G54" s="9"/>
     </row>
     <row r="55" spans="1:7" ht="15.75" customHeight="1">
       <c r="B55" s="74"/>
@@ -2487,7 +2558,7 @@
       <c r="B63" s="74"/>
       <c r="C63" s="74"/>
     </row>
-    <row r="64" spans="1:7" ht="13">
+    <row r="64" spans="1:7" ht="15.75" customHeight="1">
       <c r="B64" s="74"/>
       <c r="C64" s="74"/>
     </row>
@@ -6275,9 +6346,13 @@
       <c r="B1010" s="74"/>
       <c r="C1010" s="74"/>
     </row>
+    <row r="1011" spans="2:3" ht="13">
+      <c r="B1011" s="74"/>
+      <c r="C1011" s="74"/>
+    </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B27:E27"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="D1:E1"/>
@@ -6299,9 +6374,9 @@
     <hyperlink ref="C19" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
     <hyperlink ref="D19" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
     <hyperlink ref="E19" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="B24" r:id="rId13" xr:uid="{9D45292F-4DF7-FB46-A4BB-FE81BB0CAFD7}"/>
-    <hyperlink ref="C24" r:id="rId14" xr:uid="{7B808EA3-3AE1-3943-8E7A-54B1456282A4}"/>
-    <hyperlink ref="D24" r:id="rId15" xr:uid="{4DEB1400-E116-8A47-8E39-BA0366DC40E1}"/>
+    <hyperlink ref="B25" r:id="rId13" xr:uid="{9D45292F-4DF7-FB46-A4BB-FE81BB0CAFD7}"/>
+    <hyperlink ref="C25" r:id="rId14" xr:uid="{7B808EA3-3AE1-3943-8E7A-54B1456282A4}"/>
+    <hyperlink ref="D25" r:id="rId15" xr:uid="{4DEB1400-E116-8A47-8E39-BA0366DC40E1}"/>
     <hyperlink ref="C11" r:id="rId16" xr:uid="{FEBE3A66-3830-9040-8A39-8224B5F40D3C}"/>
     <hyperlink ref="C12" r:id="rId17" xr:uid="{2E96C83A-AC7A-3145-99A7-8C46E9E18660}"/>
     <hyperlink ref="C13" r:id="rId18" xr:uid="{484A1410-AE50-F046-A9F6-25DDF752262B}"/>
@@ -6311,6 +6386,10 @@
     <hyperlink ref="E13" r:id="rId22" xr:uid="{0CDAC340-0A45-8F41-8CF9-D804202312D5}"/>
     <hyperlink ref="E14" r:id="rId23" xr:uid="{2B07D10D-DE71-3F4B-8CD5-0423AC1A4ACE}"/>
     <hyperlink ref="B9" r:id="rId24" xr:uid="{F0D4CA2C-A633-7647-BE50-42059087D399}"/>
+    <hyperlink ref="C28" r:id="rId25" xr:uid="{A6C6C7A4-1E00-844C-B44F-2D7C11461253}"/>
+    <hyperlink ref="B28" r:id="rId26" xr:uid="{0CCDFA79-F98B-A34A-9798-3E9FDA523C0D}"/>
+    <hyperlink ref="D28" r:id="rId27" xr:uid="{087AAF6A-78D8-A042-9D61-E687DE26F2EE}"/>
+    <hyperlink ref="E28" r:id="rId28" xr:uid="{58CFA1C4-3069-B746-ACC4-532395B93FD1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6355,27 +6434,27 @@
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="E1" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="82"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="81" t="s">
+      <c r="F1" s="87"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="82"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="81" t="s">
+      <c r="I1" s="87"/>
+      <c r="J1" s="88"/>
+      <c r="K1" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="82"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="81" t="s">
+      <c r="L1" s="87"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="83"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="88"/>
       <c r="R1" s="3"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -6788,27 +6867,27 @@
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="E1" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="82"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="81" t="s">
+      <c r="F1" s="87"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="82"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="81" t="s">
+      <c r="I1" s="87"/>
+      <c r="J1" s="88"/>
+      <c r="K1" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="82"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="81" t="s">
+      <c r="L1" s="87"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="83"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="88"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1">
       <c r="A2" s="7"/>
@@ -6924,9 +7003,9 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="85"/>
-      <c r="L5" s="82"/>
-      <c r="M5" s="82"/>
+      <c r="K5" s="90"/>
+      <c r="L5" s="87"/>
+      <c r="M5" s="87"/>
       <c r="N5" s="32"/>
       <c r="O5" s="34"/>
       <c r="P5" s="34"/>
@@ -6947,9 +7026,9 @@
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="K7" s="84"/>
-      <c r="L7" s="77"/>
-      <c r="M7" s="77"/>
+      <c r="K7" s="89"/>
+      <c r="L7" s="81"/>
+      <c r="M7" s="81"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1">
       <c r="B8" s="9"/>
@@ -6971,9 +7050,9 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="K10" s="84"/>
-      <c r="L10" s="77"/>
-      <c r="M10" s="77"/>
+      <c r="K10" s="89"/>
+      <c r="L10" s="81"/>
+      <c r="M10" s="81"/>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
@@ -7004,9 +7083,9 @@
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
-      <c r="K13" s="84"/>
-      <c r="L13" s="77"/>
-      <c r="M13" s="77"/>
+      <c r="K13" s="89"/>
+      <c r="L13" s="81"/>
+      <c r="M13" s="81"/>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
@@ -7075,9 +7154,9 @@
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
-      <c r="K21" s="84"/>
-      <c r="L21" s="77"/>
-      <c r="M21" s="77"/>
+      <c r="K21" s="89"/>
+      <c r="L21" s="81"/>
+      <c r="M21" s="81"/>
     </row>
     <row r="22" spans="2:17" ht="15.75" customHeight="1">
       <c r="B22" s="9"/>
@@ -7095,9 +7174,9 @@
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
-      <c r="K23" s="84"/>
-      <c r="L23" s="77"/>
-      <c r="M23" s="77"/>
+      <c r="K23" s="89"/>
+      <c r="L23" s="81"/>
+      <c r="M23" s="81"/>
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
@@ -7242,9 +7321,9 @@
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
-      <c r="K36" s="84"/>
-      <c r="L36" s="77"/>
-      <c r="M36" s="77"/>
+      <c r="K36" s="89"/>
+      <c r="L36" s="81"/>
+      <c r="M36" s="81"/>
     </row>
     <row r="37" spans="2:17" ht="15.75" customHeight="1">
       <c r="B37" s="9"/>
@@ -7264,9 +7343,9 @@
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
-      <c r="K38" s="84"/>
-      <c r="L38" s="77"/>
-      <c r="M38" s="77"/>
+      <c r="K38" s="89"/>
+      <c r="L38" s="81"/>
+      <c r="M38" s="81"/>
       <c r="N38" s="9"/>
       <c r="O38" s="9"/>
       <c r="P38" s="9"/>
@@ -7415,12 +7494,14 @@
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
-      <c r="K51" s="84"/>
-      <c r="L51" s="77"/>
-      <c r="M51" s="77"/>
+      <c r="K51" s="89"/>
+      <c r="L51" s="81"/>
+      <c r="M51" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="K1:M1"/>
     <mergeCell ref="K51:M51"/>
     <mergeCell ref="K10:M10"/>
     <mergeCell ref="K13:M13"/>
@@ -7432,8 +7513,6 @@
     <mergeCell ref="K7:M7"/>
     <mergeCell ref="K21:M21"/>
     <mergeCell ref="K5:M5"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="K1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7482,27 +7561,27 @@
       <c r="D1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="E1" s="86" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="82"/>
-      <c r="G1" s="83"/>
-      <c r="H1" s="81" t="s">
+      <c r="F1" s="87"/>
+      <c r="G1" s="88"/>
+      <c r="H1" s="86" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="82"/>
-      <c r="J1" s="83"/>
-      <c r="K1" s="81" t="s">
+      <c r="I1" s="87"/>
+      <c r="J1" s="88"/>
+      <c r="K1" s="86" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="82"/>
-      <c r="M1" s="83"/>
-      <c r="N1" s="81" t="s">
+      <c r="L1" s="87"/>
+      <c r="M1" s="88"/>
+      <c r="N1" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="82"/>
-      <c r="P1" s="82"/>
-      <c r="Q1" s="83"/>
+      <c r="O1" s="87"/>
+      <c r="P1" s="87"/>
+      <c r="Q1" s="88"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="7"/>
@@ -7668,11 +7747,11 @@
       <c r="H6" s="27"/>
       <c r="I6" s="27"/>
       <c r="J6" s="27"/>
-      <c r="K6" s="94" t="s">
+      <c r="K6" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="L6" s="90"/>
-      <c r="M6" s="90"/>
+      <c r="L6" s="92"/>
+      <c r="M6" s="92"/>
       <c r="N6" s="18" t="s">
         <v>107</v>
       </c>
@@ -7749,11 +7828,11 @@
       <c r="H9" s="26"/>
       <c r="I9" s="27"/>
       <c r="J9" s="27"/>
-      <c r="K9" s="94" t="s">
+      <c r="K9" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="L9" s="90"/>
-      <c r="M9" s="90"/>
+      <c r="L9" s="92"/>
+      <c r="M9" s="92"/>
       <c r="N9" s="26"/>
       <c r="O9" s="27"/>
       <c r="P9" s="27"/>
@@ -7830,11 +7909,11 @@
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
       <c r="J12" s="27"/>
-      <c r="K12" s="94" t="s">
+      <c r="K12" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="L12" s="90"/>
-      <c r="M12" s="90"/>
+      <c r="L12" s="92"/>
+      <c r="M12" s="92"/>
       <c r="N12" s="18"/>
       <c r="O12" s="20"/>
       <c r="P12" s="20"/>
@@ -7897,11 +7976,11 @@
       <c r="H15" s="26"/>
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
-      <c r="K15" s="94" t="s">
+      <c r="K15" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="L15" s="90"/>
-      <c r="M15" s="90"/>
+      <c r="L15" s="92"/>
+      <c r="M15" s="92"/>
       <c r="N15" s="18" t="s">
         <v>122</v>
       </c>
@@ -8099,11 +8178,11 @@
       <c r="H23" s="26"/>
       <c r="I23" s="27"/>
       <c r="J23" s="27"/>
-      <c r="K23" s="94" t="s">
+      <c r="K23" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="L23" s="90"/>
-      <c r="M23" s="91"/>
+      <c r="L23" s="92"/>
+      <c r="M23" s="93"/>
       <c r="N23" s="26"/>
       <c r="O23" s="27"/>
       <c r="P23" s="27"/>
@@ -8144,11 +8223,11 @@
       <c r="E25" s="18"/>
       <c r="F25" s="20"/>
       <c r="G25" s="22"/>
-      <c r="K25" s="94" t="s">
+      <c r="K25" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="L25" s="90"/>
-      <c r="M25" s="91"/>
+      <c r="L25" s="92"/>
+      <c r="M25" s="93"/>
       <c r="N25" s="18" t="s">
         <v>122</v>
       </c>
@@ -8473,11 +8552,11 @@
       <c r="H38" s="26"/>
       <c r="I38" s="27"/>
       <c r="J38" s="27"/>
-      <c r="K38" s="92" t="s">
+      <c r="K38" s="98" t="s">
         <v>106</v>
       </c>
-      <c r="L38" s="77"/>
-      <c r="M38" s="93"/>
+      <c r="L38" s="81"/>
+      <c r="M38" s="99"/>
       <c r="N38" s="24"/>
       <c r="Q38" s="25"/>
       <c r="S38" s="51"/>
@@ -8527,11 +8606,11 @@
       <c r="J40" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="K40" s="94" t="s">
+      <c r="K40" s="91" t="s">
         <v>106</v>
       </c>
-      <c r="L40" s="90"/>
-      <c r="M40" s="91"/>
+      <c r="L40" s="92"/>
+      <c r="M40" s="93"/>
       <c r="N40" s="18" t="s">
         <v>122</v>
       </c>
@@ -8884,11 +8963,11 @@
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
       <c r="H53" s="24"/>
-      <c r="K53" s="92" t="s">
+      <c r="K53" s="98" t="s">
         <v>106</v>
       </c>
-      <c r="L53" s="77"/>
-      <c r="M53" s="93"/>
+      <c r="L53" s="81"/>
+      <c r="M53" s="99"/>
       <c r="N53" s="26"/>
       <c r="O53" s="27"/>
       <c r="P53" s="27"/>
@@ -8906,9 +8985,9 @@
       <c r="H54" s="30"/>
       <c r="I54" s="35"/>
       <c r="J54" s="35"/>
-      <c r="K54" s="86"/>
-      <c r="L54" s="87"/>
-      <c r="M54" s="88"/>
+      <c r="K54" s="94"/>
+      <c r="L54" s="95"/>
+      <c r="M54" s="96"/>
       <c r="N54" s="30"/>
       <c r="O54" s="35"/>
       <c r="P54" s="35"/>
@@ -8940,11 +9019,11 @@
       <c r="S57" s="51"/>
     </row>
     <row r="58" spans="1:19" ht="15.75" customHeight="1">
-      <c r="K58" s="89" t="s">
+      <c r="K58" s="97" t="s">
         <v>106</v>
       </c>
-      <c r="L58" s="90"/>
-      <c r="M58" s="91"/>
+      <c r="L58" s="92"/>
+      <c r="M58" s="93"/>
       <c r="S58" s="53"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" customHeight="1">
@@ -8983,11 +9062,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K23:M23"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="K54:M54"/>
@@ -8998,6 +9072,11 @@
     <mergeCell ref="K15:M15"/>
     <mergeCell ref="K25:M25"/>
     <mergeCell ref="K38:M38"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K23:M23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9024,12 +9103,12 @@
       <c r="A1" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="86" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="83"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="88"/>
       <c r="F1" s="49"/>
       <c r="G1" s="49"/>
       <c r="H1" s="49"/>

</xml_diff>

<commit_message>
Updates to lab environment
</commit_message>
<xml_diff>
--- a/Mifos-io-environment-details.xlsx
+++ b/Mifos-io-environment-details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sconrad/DIAL/mifos/mifos-io-configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFBFAD75-356E-5749-A435-CA5EA28AEB4D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405081F4-8165-194B-B747-D83B3A1AA597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1220" yWindow="840" windowWidth="27860" windowHeight="17580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,12 +32,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="314">
   <si>
     <t>URL</t>
-  </si>
-  <si>
-    <t>Fineract v1.2 instance 1</t>
   </si>
   <si>
     <t>Method</t>
@@ -952,6 +949,48 @@
   </si>
   <si>
     <t>https://elephant.mifos.io:8443/fineract-provider/api/v1/interoperation</t>
+  </si>
+  <si>
+    <t>Fineract CN instance 1</t>
+  </si>
+  <si>
+    <t>Fineract v1.2 instance 3</t>
+  </si>
+  <si>
+    <t>Cheetah</t>
+  </si>
+  <si>
+    <t>Giraffe</t>
+  </si>
+  <si>
+    <t>in03</t>
+  </si>
+  <si>
+    <t>tn05</t>
+  </si>
+  <si>
+    <t>tn06</t>
+  </si>
+  <si>
+    <t>in03tn05</t>
+  </si>
+  <si>
+    <t>in03tn06</t>
+  </si>
+  <si>
+    <t>fineract3.mifos.io</t>
+  </si>
+  <si>
+    <t>a545191576169183330862</t>
+  </si>
+  <si>
+    <t>b780411350952999709451</t>
+  </si>
+  <si>
+    <t>http://fineract3.mifos.io:9002/?baseApiUrl=https://fineract3.mifos.io:8443&amp;tenantIdentifier=tn05</t>
+  </si>
+  <si>
+    <t>http://fineract3.mifos.io:9002/?baseApiUrl=https://fineract3.mifos.io:8443&amp;tenantIdentifier=tn06</t>
   </si>
 </sst>
 </file>
@@ -1281,7 +1320,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="104">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1395,6 +1434,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1413,11 +1455,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1426,10 +1463,16 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1751,10 +1794,10 @@
   <dimension ref="A1:Y1011"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1763,20 +1806,23 @@
     <col min="2" max="2" width="54.6640625" customWidth="1"/>
     <col min="3" max="3" width="51.6640625" customWidth="1"/>
     <col min="4" max="5" width="47.5" customWidth="1"/>
+    <col min="6" max="7" width="47.5" style="81" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="15.75" customHeight="1">
       <c r="A1" s="1"/>
-      <c r="B1" s="83" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="81"/>
-      <c r="D1" s="84" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="81"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="86" t="s">
+        <v>300</v>
+      </c>
+      <c r="C1" s="84"/>
+      <c r="D1" s="87" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="84"/>
+      <c r="F1" s="87" t="s">
+        <v>301</v>
+      </c>
+      <c r="G1" s="84"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -1798,89 +1844,104 @@
     </row>
     <row r="2" spans="1:25" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="B2" s="88"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="84"/>
+      <c r="E2" s="84"/>
+      <c r="F2" s="84"/>
+      <c r="G2" s="84"/>
     </row>
     <row r="3" spans="1:25" ht="15.75" customHeight="1">
       <c r="A3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="11" t="s">
-        <v>12</v>
-      </c>
       <c r="C3" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="E3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="F3" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="4" spans="1:25" ht="15.75" customHeight="1">
       <c r="A4" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="83" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="80" t="s">
+      <c r="C4" s="84"/>
+      <c r="D4" s="83" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="81"/>
-      <c r="D4" s="80" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="81"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
+      <c r="E4" s="84"/>
+      <c r="F4" s="103" t="s">
+        <v>304</v>
+      </c>
+      <c r="G4" s="84"/>
     </row>
     <row r="5" spans="1:25" ht="15.75" customHeight="1">
       <c r="A5" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="C5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="D5" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="E5" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="6"/>
-      <c r="G5" s="13"/>
+      <c r="F5" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="6" spans="1:25" ht="15.75" customHeight="1">
       <c r="A6" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="C6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="D6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>32</v>
-      </c>
       <c r="E6" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="7" spans="1:25" ht="15.75" customHeight="1">
       <c r="A7" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" s="13" t="s">
         <v>269</v>
@@ -1889,203 +1950,223 @@
         <v>269</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="13"/>
+        <v>268</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>309</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="8" spans="1:25" ht="15.75" customHeight="1">
       <c r="A8" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B8" s="37"/>
       <c r="C8" s="37"/>
       <c r="D8" s="37"/>
       <c r="E8" s="37"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="39"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
     </row>
     <row r="9" spans="1:25" ht="15.75" customHeight="1">
       <c r="A9" s="42" t="s">
-        <v>75</v>
-      </c>
-      <c r="B9" s="82" t="s">
-        <v>291</v>
-      </c>
-      <c r="C9" s="81"/>
-      <c r="D9" s="81"/>
-      <c r="E9" s="81"/>
+        <v>74</v>
+      </c>
+      <c r="B9" s="85" t="s">
+        <v>290</v>
+      </c>
+      <c r="C9" s="84"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="84"/>
       <c r="F9" s="6"/>
       <c r="G9" s="39"/>
     </row>
     <row r="10" spans="1:25" ht="15.75" customHeight="1">
       <c r="A10" s="42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="37"/>
       <c r="C10" s="13" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D10" s="37"/>
       <c r="E10" s="78" t="s">
-        <v>286</v>
-      </c>
-      <c r="F10" s="6"/>
-      <c r="G10" s="39"/>
+        <v>285</v>
+      </c>
+      <c r="F10" s="37"/>
+      <c r="G10" s="78"/>
     </row>
     <row r="11" spans="1:25" ht="15.75" customHeight="1">
       <c r="A11" s="42" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B11" s="37"/>
       <c r="C11" s="75" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D11" s="37"/>
       <c r="E11" s="75" t="s">
-        <v>287</v>
-      </c>
-      <c r="F11" s="6"/>
-      <c r="G11" s="39"/>
+        <v>286</v>
+      </c>
+      <c r="F11" s="37"/>
+      <c r="G11" s="82"/>
     </row>
     <row r="12" spans="1:25" ht="15.75" customHeight="1">
       <c r="A12" s="42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" s="37"/>
       <c r="C12" s="75" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D12" s="37"/>
       <c r="E12" s="75" t="s">
-        <v>288</v>
-      </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="39"/>
+        <v>287</v>
+      </c>
+      <c r="F12" s="37"/>
+      <c r="G12" s="82"/>
     </row>
     <row r="13" spans="1:25" ht="15.75" customHeight="1">
       <c r="A13" s="42" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B13" s="37"/>
       <c r="C13" s="75" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D13" s="37"/>
       <c r="E13" s="75" t="s">
-        <v>289</v>
-      </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="39"/>
+        <v>288</v>
+      </c>
+      <c r="F13" s="37"/>
+      <c r="G13" s="82"/>
     </row>
     <row r="14" spans="1:25" ht="15.75" customHeight="1">
       <c r="A14" s="31" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B14" s="21"/>
       <c r="C14" s="75" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D14" s="13"/>
       <c r="E14" s="75" t="s">
-        <v>290</v>
-      </c>
-      <c r="F14" s="6"/>
-      <c r="G14" s="39"/>
+        <v>289</v>
+      </c>
+      <c r="F14" s="13"/>
+      <c r="G14" s="82"/>
     </row>
     <row r="15" spans="1:25" ht="15.75" customHeight="1">
       <c r="A15" s="42" t="s">
+        <v>209</v>
+      </c>
+      <c r="B15" s="11" t="s">
         <v>210</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="C15" s="11" t="s">
         <v>211</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>212</v>
-      </c>
       <c r="D15" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="E15" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="F15" s="80" t="s">
+        <v>210</v>
+      </c>
+      <c r="G15" s="80" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="16" spans="1:25" ht="15.75" customHeight="1">
       <c r="A16" s="42" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B16" s="11"/>
       <c r="C16" s="11"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="80"/>
     </row>
     <row r="17" spans="1:25" ht="15.75" customHeight="1">
       <c r="A17" s="31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B17" s="75" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C17" s="75" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D17" s="75" t="s">
+        <v>277</v>
+      </c>
+      <c r="E17" s="75" t="s">
         <v>278</v>
       </c>
-      <c r="E17" s="75" t="s">
-        <v>279</v>
-      </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="F17" s="82" t="s">
+        <v>312</v>
+      </c>
+      <c r="G17" s="82" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="18" spans="1:25" ht="15.75" customHeight="1">
       <c r="A18" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="F18" s="6"/>
-      <c r="G18" s="13"/>
+        <v>247</v>
+      </c>
+      <c r="F18" s="80" t="s">
+        <v>247</v>
+      </c>
+      <c r="G18" s="80" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="19" spans="1:25" ht="15.75" customHeight="1">
       <c r="A19" s="68" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B19" s="79" t="s">
+        <v>273</v>
+      </c>
+      <c r="C19" s="79" t="s">
         <v>274</v>
       </c>
-      <c r="C19" s="79" t="s">
-        <v>275</v>
-      </c>
       <c r="D19" s="79" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E19" s="79" t="s">
-        <v>280</v>
-      </c>
-      <c r="F19" s="6"/>
-      <c r="G19" s="70"/>
+        <v>279</v>
+      </c>
+      <c r="F19" s="82" t="s">
+        <v>276</v>
+      </c>
+      <c r="G19" s="82" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="20" spans="1:25" ht="15.75" customHeight="1">
       <c r="A20" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B20" s="71">
         <v>27710101999</v>
@@ -2099,46 +2180,58 @@
       <c r="E20" s="39">
         <v>27710204999</v>
       </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
+      <c r="F20" s="71">
+        <v>27710203999</v>
+      </c>
+      <c r="G20" s="71">
+        <v>27710204999</v>
+      </c>
     </row>
     <row r="21" spans="1:25" ht="15.75" customHeight="1">
       <c r="A21" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="B21" s="9" t="s">
         <v>256</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="C21" s="9" t="s">
         <v>257</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="D21" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="E21" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="E21" s="6" t="s">
-        <v>260</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="13"/>
+      <c r="F21" s="80" t="s">
+        <v>258</v>
+      </c>
+      <c r="G21" s="80" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="22" spans="1:25" ht="15.75" customHeight="1">
       <c r="A22" s="72" t="s">
+        <v>260</v>
+      </c>
+      <c r="B22" s="11" t="s">
         <v>261</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="C22" s="11" t="s">
         <v>262</v>
       </c>
-      <c r="C22" s="11" t="s">
-        <v>263</v>
-      </c>
       <c r="D22" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="E22" s="6" t="s">
         <v>262</v>
       </c>
-      <c r="E22" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
+      <c r="F22" s="80" t="s">
+        <v>261</v>
+      </c>
+      <c r="G22" s="80" t="s">
+        <v>262</v>
+      </c>
       <c r="H22" s="6"/>
       <c r="I22" s="6"/>
       <c r="J22" s="6"/>
@@ -2160,22 +2253,26 @@
     </row>
     <row r="23" spans="1:25" ht="15.75" customHeight="1">
       <c r="A23" s="72" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B23" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>294</v>
       </c>
-      <c r="C23" s="9" t="s">
-        <v>292</v>
-      </c>
-      <c r="D23" s="9" t="s">
+      <c r="E23" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="E23" s="9" t="s">
-        <v>296</v>
-      </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
+      <c r="F23" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>311</v>
+      </c>
       <c r="H23" s="6"/>
       <c r="I23" s="6"/>
       <c r="J23" s="6"/>
@@ -2197,7 +2294,7 @@
     </row>
     <row r="24" spans="1:25" s="77" customFormat="1" ht="15.75" customHeight="1">
       <c r="A24" s="9" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B24" s="9">
         <v>1</v>
@@ -2211,8 +2308,12 @@
       <c r="E24" s="76">
         <v>1</v>
       </c>
-      <c r="F24" s="76"/>
-      <c r="G24" s="76"/>
+      <c r="F24" s="9">
+        <v>1</v>
+      </c>
+      <c r="G24" s="80">
+        <v>1</v>
+      </c>
       <c r="H24" s="76"/>
       <c r="I24" s="76"/>
       <c r="J24" s="76"/>
@@ -2234,59 +2335,71 @@
     </row>
     <row r="25" spans="1:25" ht="15.75" customHeight="1">
       <c r="A25" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B25" s="75" t="s">
+        <v>270</v>
+      </c>
+      <c r="C25" s="75" t="s">
+        <v>270</v>
+      </c>
+      <c r="D25" s="75" t="s">
         <v>271</v>
       </c>
-      <c r="C25" s="75" t="s">
+      <c r="E25" s="13" t="s">
         <v>271</v>
       </c>
-      <c r="D25" s="75" t="s">
-        <v>272</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>272</v>
-      </c>
-      <c r="F25" s="6"/>
+      <c r="F25" s="82" t="s">
+        <v>271</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="26" spans="1:25" ht="15.75" customHeight="1">
       <c r="A26" s="9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B26" s="73"/>
       <c r="C26" s="21"/>
       <c r="D26" s="70"/>
       <c r="E26" s="70"/>
-      <c r="F26" s="6"/>
+      <c r="F26" s="70"/>
+      <c r="G26" s="70"/>
     </row>
     <row r="27" spans="1:25" ht="15.75" customHeight="1">
       <c r="A27" s="9" t="s">
-        <v>267</v>
-      </c>
-      <c r="B27" s="80"/>
-      <c r="C27" s="81"/>
-      <c r="D27" s="81"/>
-      <c r="E27" s="81"/>
+        <v>266</v>
+      </c>
+      <c r="B27" s="83"/>
+      <c r="C27" s="84"/>
+      <c r="D27" s="84"/>
+      <c r="E27" s="84"/>
       <c r="F27" s="6"/>
+      <c r="G27"/>
     </row>
     <row r="28" spans="1:25" ht="15.75" customHeight="1">
       <c r="A28" s="9" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B28" s="79" t="s">
+        <v>297</v>
+      </c>
+      <c r="C28" s="79" t="s">
+        <v>296</v>
+      </c>
+      <c r="D28" s="79" t="s">
         <v>298</v>
       </c>
-      <c r="C28" s="79" t="s">
-        <v>297</v>
-      </c>
-      <c r="D28" s="79" t="s">
+      <c r="E28" s="79" t="s">
         <v>299</v>
       </c>
-      <c r="E28" s="79" t="s">
-        <v>300</v>
-      </c>
-      <c r="F28" s="6"/>
+      <c r="F28" s="82" t="s">
+        <v>298</v>
+      </c>
+      <c r="G28" s="82" t="s">
+        <v>299</v>
+      </c>
     </row>
     <row r="29" spans="1:25" ht="15.75" customHeight="1">
       <c r="A29" s="9"/>
@@ -6351,7 +6464,10 @@
       <c r="C1011" s="74"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="11">
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F4:G4"/>
     <mergeCell ref="B27:E27"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B1:C1"/>
@@ -6390,6 +6506,15 @@
     <hyperlink ref="B28" r:id="rId26" xr:uid="{0CCDFA79-F98B-A34A-9798-3E9FDA523C0D}"/>
     <hyperlink ref="D28" r:id="rId27" xr:uid="{087AAF6A-78D8-A042-9D61-E687DE26F2EE}"/>
     <hyperlink ref="E28" r:id="rId28" xr:uid="{58CFA1C4-3069-B746-ACC4-532395B93FD1}"/>
+    <hyperlink ref="F7" r:id="rId29" display="rhino.mlabs.dpc.hu" xr:uid="{60740827-DDE2-4043-A90C-AF115613A475}"/>
+    <hyperlink ref="G7" r:id="rId30" display="elephant.mlabs.dpc.hu" xr:uid="{57E7FBA5-37E5-A84A-B8F2-6C4AAF12DE39}"/>
+    <hyperlink ref="F17" r:id="rId31" xr:uid="{C7C634E2-4B08-1B4B-BB03-3B221F292D96}"/>
+    <hyperlink ref="G17" r:id="rId32" xr:uid="{F9E05D81-8BA2-4B44-A975-2ECD8A56D77F}"/>
+    <hyperlink ref="F19" r:id="rId33" xr:uid="{4BE9D7D8-881B-5048-814B-24C244C5635A}"/>
+    <hyperlink ref="G19" r:id="rId34" xr:uid="{12D77A67-ABE2-5140-8AA0-3FB4776E5098}"/>
+    <hyperlink ref="F25" r:id="rId35" xr:uid="{E3F7CD8E-6CC9-DB49-AF54-B1C5250E5C19}"/>
+    <hyperlink ref="F28" r:id="rId36" xr:uid="{D015083F-7166-964B-891A-362371B8E696}"/>
+    <hyperlink ref="G28" r:id="rId37" xr:uid="{10B28FE3-1296-5B4C-ACBA-40A3F51BA3A3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6426,35 +6551,35 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="86" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="87"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="86" t="s">
+      <c r="F1" s="90"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="89" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="90"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="87"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="86" t="s">
+      <c r="L1" s="90"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="87"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="86" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="88"/>
+      <c r="O1" s="90"/>
+      <c r="P1" s="90"/>
+      <c r="Q1" s="91"/>
       <c r="R1" s="3"/>
       <c r="S1" s="1"/>
       <c r="T1" s="1"/>
@@ -6483,43 +6608,43 @@
       <c r="C2" s="8"/>
       <c r="D2" s="10"/>
       <c r="E2" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>21</v>
-      </c>
       <c r="P2" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -6545,16 +6670,16 @@
     </row>
     <row r="3" spans="1:38" ht="15.75" customHeight="1">
       <c r="A3" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>35</v>
-      </c>
-      <c r="D3" s="15" t="s">
-        <v>36</v>
       </c>
       <c r="E3" s="17"/>
       <c r="F3" s="9"/>
@@ -6563,25 +6688,25 @@
       <c r="I3" s="9"/>
       <c r="J3" s="19"/>
       <c r="K3" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="L3" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="L3" s="9" t="s">
+      <c r="M3" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="M3" s="19" t="s">
+      <c r="N3" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="N3" s="17" t="s">
+      <c r="O3" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="O3" s="9" t="s">
+      <c r="P3" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="P3" s="9" t="s">
+      <c r="Q3" s="19" t="s">
         <v>44</v>
-      </c>
-      <c r="Q3" s="19" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:38" ht="15.75" customHeight="1">
@@ -6596,21 +6721,21 @@
       <c r="K4" s="24"/>
       <c r="M4" s="25"/>
       <c r="N4" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O4" s="9">
         <v>1</v>
       </c>
       <c r="P4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="Q4" s="19" t="s">
         <v>47</v>
-      </c>
-      <c r="Q4" s="19" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:38" ht="15.75" customHeight="1">
       <c r="A5" s="28" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="23"/>
       <c r="C5" s="23"/>
@@ -6622,21 +6747,21 @@
       <c r="K5" s="24"/>
       <c r="M5" s="25"/>
       <c r="N5" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O5" s="9">
         <v>1</v>
       </c>
       <c r="P5" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Q5" s="19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:38" ht="15.75" customHeight="1">
       <c r="A6" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B6" s="23"/>
       <c r="C6" s="23"/>
@@ -6648,21 +6773,21 @@
       <c r="K6" s="24"/>
       <c r="M6" s="25"/>
       <c r="N6" s="17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O6" s="9">
         <v>1</v>
       </c>
       <c r="P6" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q6" s="19" t="s">
         <v>56</v>
-      </c>
-      <c r="Q6" s="19" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:38" ht="15.75" customHeight="1">
       <c r="A7" s="28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" s="23"/>
       <c r="C7" s="23"/>
@@ -6674,21 +6799,21 @@
       <c r="K7" s="24"/>
       <c r="M7" s="25"/>
       <c r="N7" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O7" s="9">
         <v>1</v>
       </c>
       <c r="P7" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q7" s="19" t="s">
         <v>61</v>
-      </c>
-      <c r="Q7" s="19" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:38" ht="15.75" customHeight="1">
       <c r="A8" s="28" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="23"/>
       <c r="C8" s="23"/>
@@ -6700,21 +6825,21 @@
       <c r="K8" s="24"/>
       <c r="M8" s="25"/>
       <c r="N8" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O8" s="9">
         <v>1</v>
       </c>
       <c r="P8" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q8" s="19" t="s">
         <v>66</v>
-      </c>
-      <c r="Q8" s="19" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="9" spans="1:38" ht="15.75" customHeight="1">
       <c r="A9" s="28" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B9" s="23"/>
       <c r="C9" s="23"/>
@@ -6726,16 +6851,16 @@
       <c r="K9" s="24"/>
       <c r="M9" s="25"/>
       <c r="N9" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="O9" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P9" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="O9" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="P9" s="9" t="s">
+      <c r="Q9" s="19" t="s">
         <v>70</v>
-      </c>
-      <c r="Q9" s="19" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:38" ht="15.75" customHeight="1">
@@ -6753,37 +6878,37 @@
       <c r="L10" s="35"/>
       <c r="M10" s="36"/>
       <c r="N10" s="38" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O10" s="40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P10" s="40" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q10" s="41" t="s">
         <v>76</v>
-      </c>
-      <c r="Q10" s="41" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:38" ht="15.75" customHeight="1">
       <c r="A11" s="23"/>
       <c r="B11" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="C11" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="C11" s="43" t="s">
+      <c r="D11" s="43" t="s">
         <v>79</v>
       </c>
-      <c r="D11" s="43" t="s">
+      <c r="E11" s="34" t="s">
         <v>80</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="F11" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="F11" s="34" t="s">
+      <c r="G11" s="44" t="s">
         <v>82</v>
-      </c>
-      <c r="G11" s="44" t="s">
-        <v>83</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
@@ -6799,22 +6924,22 @@
     <row r="12" spans="1:38" ht="15.75" customHeight="1">
       <c r="A12" s="33"/>
       <c r="B12" s="43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C12" s="43" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="43" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="43" t="s">
+      <c r="E12" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="34" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="44" t="s">
         <v>86</v>
-      </c>
-      <c r="E12" s="34" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="G12" s="44" t="s">
-        <v>87</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
@@ -6859,35 +6984,35 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="86" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="87"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="86" t="s">
+      <c r="F1" s="90"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="89" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="90"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="87"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="86" t="s">
+      <c r="L1" s="90"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="87"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="86" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="88"/>
+      <c r="O1" s="90"/>
+      <c r="P1" s="90"/>
+      <c r="Q1" s="91"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" customHeight="1">
       <c r="A2" s="7"/>
@@ -6895,57 +7020,57 @@
       <c r="C2" s="8"/>
       <c r="D2" s="12"/>
       <c r="E2" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>21</v>
-      </c>
       <c r="P2" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" customHeight="1">
       <c r="A3" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="14" t="s">
         <v>37</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>38</v>
       </c>
       <c r="E3" s="18"/>
       <c r="F3" s="20"/>
@@ -6964,13 +7089,13 @@
     <row r="4" spans="1:17" ht="15.75" customHeight="1">
       <c r="A4" s="23"/>
       <c r="B4" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="18" t="s">
         <v>49</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>50</v>
       </c>
       <c r="E4" s="18"/>
       <c r="F4" s="20"/>
@@ -6989,13 +7114,13 @@
     <row r="5" spans="1:17" ht="15.75" customHeight="1">
       <c r="A5" s="30"/>
       <c r="B5" s="32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="32" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="32" t="s">
         <v>72</v>
-      </c>
-      <c r="D5" s="32" t="s">
-        <v>73</v>
       </c>
       <c r="E5" s="32"/>
       <c r="F5" s="34"/>
@@ -7003,9 +7128,9 @@
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
-      <c r="K5" s="90"/>
-      <c r="L5" s="87"/>
-      <c r="M5" s="87"/>
+      <c r="K5" s="93"/>
+      <c r="L5" s="90"/>
+      <c r="M5" s="90"/>
       <c r="N5" s="32"/>
       <c r="O5" s="34"/>
       <c r="P5" s="34"/>
@@ -7026,9 +7151,9 @@
       <c r="E7" s="9"/>
       <c r="F7" s="9"/>
       <c r="G7" s="9"/>
-      <c r="K7" s="89"/>
-      <c r="L7" s="81"/>
-      <c r="M7" s="81"/>
+      <c r="K7" s="92"/>
+      <c r="L7" s="84"/>
+      <c r="M7" s="84"/>
     </row>
     <row r="8" spans="1:17" ht="15.75" customHeight="1">
       <c r="B8" s="9"/>
@@ -7050,9 +7175,9 @@
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
-      <c r="K10" s="89"/>
-      <c r="L10" s="81"/>
-      <c r="M10" s="81"/>
+      <c r="K10" s="92"/>
+      <c r="L10" s="84"/>
+      <c r="M10" s="84"/>
       <c r="N10" s="9"/>
       <c r="O10" s="9"/>
       <c r="P10" s="9"/>
@@ -7083,9 +7208,9 @@
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
       <c r="G13" s="9"/>
-      <c r="K13" s="89"/>
-      <c r="L13" s="81"/>
-      <c r="M13" s="81"/>
+      <c r="K13" s="92"/>
+      <c r="L13" s="84"/>
+      <c r="M13" s="84"/>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
       <c r="P13" s="9"/>
@@ -7154,9 +7279,9 @@
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
       <c r="G21" s="9"/>
-      <c r="K21" s="89"/>
-      <c r="L21" s="81"/>
-      <c r="M21" s="81"/>
+      <c r="K21" s="92"/>
+      <c r="L21" s="84"/>
+      <c r="M21" s="84"/>
     </row>
     <row r="22" spans="2:17" ht="15.75" customHeight="1">
       <c r="B22" s="9"/>
@@ -7174,9 +7299,9 @@
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
       <c r="G23" s="9"/>
-      <c r="K23" s="89"/>
-      <c r="L23" s="81"/>
-      <c r="M23" s="81"/>
+      <c r="K23" s="92"/>
+      <c r="L23" s="84"/>
+      <c r="M23" s="84"/>
       <c r="N23" s="9"/>
       <c r="O23" s="9"/>
       <c r="P23" s="9"/>
@@ -7321,9 +7446,9 @@
       <c r="B36" s="9"/>
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
-      <c r="K36" s="89"/>
-      <c r="L36" s="81"/>
-      <c r="M36" s="81"/>
+      <c r="K36" s="92"/>
+      <c r="L36" s="84"/>
+      <c r="M36" s="84"/>
     </row>
     <row r="37" spans="2:17" ht="15.75" customHeight="1">
       <c r="B37" s="9"/>
@@ -7343,9 +7468,9 @@
       <c r="H38" s="9"/>
       <c r="I38" s="9"/>
       <c r="J38" s="9"/>
-      <c r="K38" s="89"/>
-      <c r="L38" s="81"/>
-      <c r="M38" s="81"/>
+      <c r="K38" s="92"/>
+      <c r="L38" s="84"/>
+      <c r="M38" s="84"/>
       <c r="N38" s="9"/>
       <c r="O38" s="9"/>
       <c r="P38" s="9"/>
@@ -7494,17 +7619,12 @@
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
       <c r="E51" s="9"/>
-      <c r="K51" s="89"/>
-      <c r="L51" s="81"/>
-      <c r="M51" s="81"/>
+      <c r="K51" s="92"/>
+      <c r="L51" s="84"/>
+      <c r="M51" s="84"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="K51:M51"/>
-    <mergeCell ref="K10:M10"/>
-    <mergeCell ref="K13:M13"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="K23:M23"/>
@@ -7513,6 +7633,11 @@
     <mergeCell ref="K7:M7"/>
     <mergeCell ref="K21:M21"/>
     <mergeCell ref="K5:M5"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="K51:M51"/>
+    <mergeCell ref="K10:M10"/>
+    <mergeCell ref="K13:M13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7553,35 +7678,35 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="86" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="87"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="86" t="s">
+      <c r="F1" s="90"/>
+      <c r="G1" s="91"/>
+      <c r="H1" s="89" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="90"/>
+      <c r="J1" s="91"/>
+      <c r="K1" s="89" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="87"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="86" t="s">
+      <c r="L1" s="90"/>
+      <c r="M1" s="91"/>
+      <c r="N1" s="89" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="87"/>
-      <c r="M1" s="88"/>
-      <c r="N1" s="86" t="s">
-        <v>10</v>
-      </c>
-      <c r="O1" s="87"/>
-      <c r="P1" s="87"/>
-      <c r="Q1" s="88"/>
+      <c r="O1" s="90"/>
+      <c r="P1" s="90"/>
+      <c r="Q1" s="91"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="7"/>
@@ -7589,43 +7714,43 @@
       <c r="C2" s="8"/>
       <c r="D2" s="12"/>
       <c r="E2" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="L2" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="N2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="O2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="L2" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>21</v>
-      </c>
       <c r="P2" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
@@ -7639,16 +7764,16 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B3" s="16" t="s">
-        <v>78</v>
-      </c>
-      <c r="C3" s="16" t="s">
+      <c r="D3" s="14" t="s">
         <v>90</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>91</v>
       </c>
       <c r="E3" s="18"/>
       <c r="F3" s="20"/>
@@ -7667,34 +7792,34 @@
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
       <c r="A4" s="23"/>
       <c r="B4" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="18" t="s">
         <v>92</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>93</v>
       </c>
       <c r="E4" s="18"/>
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
       <c r="H4" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="J4" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="I4" s="27" t="s">
+      <c r="K4" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="L4" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="27" t="s">
         <v>40</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="K4" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="L4" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="M4" s="27" t="s">
-        <v>41</v>
       </c>
       <c r="N4" s="26"/>
       <c r="O4" s="27"/>
@@ -7703,7 +7828,7 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
       <c r="A5" s="28" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B5" s="15"/>
       <c r="C5" s="17"/>
@@ -7712,13 +7837,13 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
       <c r="H5" s="24" t="s">
+        <v>98</v>
+      </c>
+      <c r="I5" t="s">
+        <v>39</v>
+      </c>
+      <c r="J5" s="9" t="s">
         <v>99</v>
-      </c>
-      <c r="I5" t="s">
-        <v>40</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>100</v>
       </c>
       <c r="K5" s="24"/>
       <c r="N5" s="24"/>
@@ -7727,42 +7852,42 @@
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
       <c r="A6" s="24"/>
       <c r="B6" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C6" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="E6" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="F6" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="F6" s="20" t="s">
+      <c r="G6" s="22" t="s">
         <v>104</v>
-      </c>
-      <c r="G6" s="22" t="s">
-        <v>105</v>
       </c>
       <c r="H6" s="27"/>
       <c r="I6" s="27"/>
       <c r="J6" s="27"/>
-      <c r="K6" s="91" t="s">
+      <c r="K6" s="102" t="s">
+        <v>105</v>
+      </c>
+      <c r="L6" s="98"/>
+      <c r="M6" s="98"/>
+      <c r="N6" s="18" t="s">
         <v>106</v>
-      </c>
-      <c r="L6" s="92"/>
-      <c r="M6" s="92"/>
-      <c r="N6" s="18" t="s">
-        <v>107</v>
       </c>
       <c r="O6" s="20">
         <v>1</v>
       </c>
       <c r="P6" s="20" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q6" s="22" t="s">
         <v>108</v>
-      </c>
-      <c r="Q6" s="22" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
@@ -7771,13 +7896,13 @@
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
       <c r="E7" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F7" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="G7" s="19" t="s">
         <v>111</v>
-      </c>
-      <c r="G7" s="19" t="s">
-        <v>112</v>
       </c>
       <c r="K7" s="17"/>
       <c r="N7" s="17"/>
@@ -7786,20 +7911,20 @@
     <row r="8" spans="1:26" ht="15.75" customHeight="1">
       <c r="A8" s="23"/>
       <c r="B8" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G8" s="19" t="s">
         <v>114</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>115</v>
       </c>
       <c r="K8" s="24"/>
       <c r="N8" s="17"/>
@@ -7808,31 +7933,31 @@
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
       <c r="A9" s="24"/>
       <c r="B9" s="14" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E9" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F9" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="F9" s="20" t="s">
+      <c r="G9" s="20" t="s">
         <v>104</v>
-      </c>
-      <c r="G9" s="20" t="s">
-        <v>105</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="27"/>
       <c r="J9" s="27"/>
-      <c r="K9" s="91" t="s">
-        <v>106</v>
-      </c>
-      <c r="L9" s="92"/>
-      <c r="M9" s="92"/>
+      <c r="K9" s="102" t="s">
+        <v>105</v>
+      </c>
+      <c r="L9" s="98"/>
+      <c r="M9" s="98"/>
       <c r="N9" s="26"/>
       <c r="O9" s="27"/>
       <c r="P9" s="27"/>
@@ -7844,13 +7969,13 @@
       <c r="C10" s="41"/>
       <c r="D10" s="9"/>
       <c r="E10" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F10" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="G10" s="9" t="s">
         <v>111</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>112</v>
       </c>
       <c r="H10" s="24"/>
       <c r="K10" s="24"/>
@@ -7860,20 +7985,20 @@
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
       <c r="A11" s="23"/>
       <c r="B11" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C11" s="38" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D11" s="38"/>
       <c r="E11" s="38" t="s">
+        <v>113</v>
+      </c>
+      <c r="F11" s="40" t="s">
+        <v>110</v>
+      </c>
+      <c r="G11" s="40" t="s">
         <v>114</v>
-      </c>
-      <c r="F11" s="40" t="s">
-        <v>111</v>
-      </c>
-      <c r="G11" s="40" t="s">
-        <v>115</v>
       </c>
       <c r="H11" s="30"/>
       <c r="I11" s="35"/>
@@ -7889,31 +8014,31 @@
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
       <c r="A12" s="24"/>
       <c r="B12" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D12" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="C12" s="18" t="s">
-        <v>101</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>118</v>
-      </c>
       <c r="E12" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="F12" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="F12" s="20" t="s">
+      <c r="G12" s="22" t="s">
         <v>104</v>
-      </c>
-      <c r="G12" s="22" t="s">
-        <v>105</v>
       </c>
       <c r="H12" s="27"/>
       <c r="I12" s="27"/>
       <c r="J12" s="27"/>
-      <c r="K12" s="91" t="s">
-        <v>106</v>
-      </c>
-      <c r="L12" s="92"/>
-      <c r="M12" s="92"/>
+      <c r="K12" s="102" t="s">
+        <v>105</v>
+      </c>
+      <c r="L12" s="98"/>
+      <c r="M12" s="98"/>
       <c r="N12" s="18"/>
       <c r="O12" s="20"/>
       <c r="P12" s="20"/>
@@ -7925,13 +8050,13 @@
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
       <c r="E13" s="17" t="s">
+        <v>109</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="G13" s="19" t="s">
         <v>111</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>112</v>
       </c>
       <c r="K13" s="17"/>
       <c r="N13" s="17"/>
@@ -7940,20 +8065,20 @@
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
       <c r="A14" s="23"/>
       <c r="B14" s="14" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C14" s="18" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D14" s="17"/>
       <c r="E14" s="17" t="s">
+        <v>113</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="G14" s="19" t="s">
         <v>114</v>
-      </c>
-      <c r="F14" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>115</v>
       </c>
       <c r="K14" s="24"/>
       <c r="N14" s="17"/>
@@ -7962,13 +8087,13 @@
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
       <c r="A15" s="24"/>
       <c r="B15" s="18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C15" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E15" s="18"/>
       <c r="F15" s="20"/>
@@ -7976,22 +8101,22 @@
       <c r="H15" s="26"/>
       <c r="I15" s="27"/>
       <c r="J15" s="27"/>
-      <c r="K15" s="91" t="s">
-        <v>106</v>
-      </c>
-      <c r="L15" s="92"/>
-      <c r="M15" s="92"/>
+      <c r="K15" s="102" t="s">
+        <v>105</v>
+      </c>
+      <c r="L15" s="98"/>
+      <c r="M15" s="98"/>
       <c r="N15" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O15" s="20">
         <v>1</v>
       </c>
       <c r="P15" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q15" s="22" t="s">
         <v>82</v>
-      </c>
-      <c r="Q15" s="22" t="s">
-        <v>83</v>
       </c>
       <c r="S15" s="50"/>
     </row>
@@ -8005,16 +8130,16 @@
       <c r="H16" s="24"/>
       <c r="K16" s="24"/>
       <c r="N16" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O16" s="9">
         <v>1</v>
       </c>
       <c r="P16" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q16" s="19" t="s">
         <v>108</v>
-      </c>
-      <c r="Q16" s="19" t="s">
-        <v>109</v>
       </c>
       <c r="S16" s="51"/>
     </row>
@@ -8028,16 +8153,16 @@
       <c r="H17" s="24"/>
       <c r="K17" s="24"/>
       <c r="N17" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O17" s="9">
         <v>1</v>
       </c>
       <c r="P17" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q17" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="S17" s="53"/>
     </row>
@@ -8051,16 +8176,16 @@
       <c r="H18" s="24"/>
       <c r="K18" s="24"/>
       <c r="N18" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O18" s="9">
         <v>1</v>
       </c>
       <c r="P18" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q18" s="19" t="s">
         <v>66</v>
-      </c>
-      <c r="Q18" s="19" t="s">
-        <v>67</v>
       </c>
       <c r="S18" s="51"/>
     </row>
@@ -8074,16 +8199,16 @@
       <c r="H19" s="24"/>
       <c r="K19" s="24"/>
       <c r="N19" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="O19" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P19" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="O19" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="P19" s="9" t="s">
-        <v>70</v>
-      </c>
       <c r="Q19" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="S19" s="54"/>
     </row>
@@ -8097,16 +8222,16 @@
       <c r="H20" s="24"/>
       <c r="K20" s="24"/>
       <c r="N20" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="O20" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P20" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="O20" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="P20" s="9" t="s">
+      <c r="Q20" s="19" t="s">
         <v>155</v>
-      </c>
-      <c r="Q20" s="19" t="s">
-        <v>156</v>
       </c>
       <c r="S20" s="51"/>
     </row>
@@ -8120,16 +8245,16 @@
       <c r="H21" s="24"/>
       <c r="K21" s="24"/>
       <c r="N21" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O21" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P21" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q21" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S21" s="54"/>
     </row>
@@ -8143,46 +8268,46 @@
       <c r="H22" s="24"/>
       <c r="K22" s="24"/>
       <c r="N22" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O22" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P22" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q22" s="19" t="s">
         <v>164</v>
-      </c>
-      <c r="Q22" s="19" t="s">
-        <v>165</v>
       </c>
       <c r="S22" s="53"/>
     </row>
     <row r="23" spans="2:19" ht="15.75" customHeight="1">
       <c r="B23" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C23" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="D23" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="D23" s="18" t="s">
-        <v>167</v>
-      </c>
       <c r="E23" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F23" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="G23" s="20" t="s">
         <v>82</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>83</v>
       </c>
       <c r="H23" s="26"/>
       <c r="I23" s="27"/>
       <c r="J23" s="27"/>
-      <c r="K23" s="91" t="s">
-        <v>106</v>
-      </c>
-      <c r="L23" s="92"/>
-      <c r="M23" s="93"/>
+      <c r="K23" s="102" t="s">
+        <v>105</v>
+      </c>
+      <c r="L23" s="98"/>
+      <c r="M23" s="99"/>
       <c r="N23" s="26"/>
       <c r="O23" s="27"/>
       <c r="P23" s="27"/>
@@ -8194,13 +8319,13 @@
       <c r="C24" s="38"/>
       <c r="D24" s="38"/>
       <c r="E24" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G24" s="9" t="s">
         <v>174</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>175</v>
       </c>
       <c r="H24" s="30"/>
       <c r="I24" s="35"/>
@@ -8214,31 +8339,31 @@
     </row>
     <row r="25" spans="2:19" ht="15.75" customHeight="1">
       <c r="B25" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D25" s="17"/>
       <c r="E25" s="18"/>
       <c r="F25" s="20"/>
       <c r="G25" s="22"/>
-      <c r="K25" s="91" t="s">
-        <v>106</v>
-      </c>
-      <c r="L25" s="92"/>
-      <c r="M25" s="93"/>
+      <c r="K25" s="102" t="s">
+        <v>105</v>
+      </c>
+      <c r="L25" s="98"/>
+      <c r="M25" s="99"/>
       <c r="N25" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O25" s="20">
         <v>1</v>
       </c>
       <c r="P25" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q25" s="22" t="s">
         <v>82</v>
-      </c>
-      <c r="Q25" s="22" t="s">
-        <v>83</v>
       </c>
       <c r="S25" s="53"/>
     </row>
@@ -8253,16 +8378,16 @@
       <c r="L26" s="46"/>
       <c r="M26" s="46"/>
       <c r="N26" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="O26" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P26" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q26" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="S26" s="50"/>
     </row>
@@ -8277,16 +8402,16 @@
       <c r="L27" s="46"/>
       <c r="M27" s="46"/>
       <c r="N27" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O27" s="9">
         <v>1</v>
       </c>
       <c r="P27" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q27" s="19" t="s">
         <v>108</v>
-      </c>
-      <c r="Q27" s="19" t="s">
-        <v>109</v>
       </c>
       <c r="S27" s="51"/>
     </row>
@@ -8301,16 +8426,16 @@
       <c r="L28" s="46"/>
       <c r="M28" s="46"/>
       <c r="N28" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O28" s="9">
         <v>1</v>
       </c>
       <c r="P28" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q28" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="S28" s="54"/>
     </row>
@@ -8325,16 +8450,16 @@
       <c r="L29" s="46"/>
       <c r="M29" s="46"/>
       <c r="N29" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O29" s="9">
         <v>1</v>
       </c>
       <c r="P29" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q29" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="S29" s="51"/>
     </row>
@@ -8349,16 +8474,16 @@
       <c r="L30" s="46"/>
       <c r="M30" s="46"/>
       <c r="N30" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O30" s="9">
         <v>1</v>
       </c>
       <c r="P30" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q30" s="19" t="s">
         <v>66</v>
-      </c>
-      <c r="Q30" s="19" t="s">
-        <v>67</v>
       </c>
       <c r="S30" s="53"/>
     </row>
@@ -8373,16 +8498,16 @@
       <c r="L31" s="46"/>
       <c r="M31" s="46"/>
       <c r="N31" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="O31" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P31" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="O31" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="P31" s="9" t="s">
-        <v>70</v>
-      </c>
       <c r="Q31" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="S31" s="52"/>
     </row>
@@ -8397,16 +8522,16 @@
       <c r="L32" s="46"/>
       <c r="M32" s="46"/>
       <c r="N32" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="O32" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P32" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="O32" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="P32" s="9" t="s">
+      <c r="Q32" s="19" t="s">
         <v>155</v>
-      </c>
-      <c r="Q32" s="19" t="s">
-        <v>156</v>
       </c>
       <c r="S32" s="53"/>
     </row>
@@ -8421,16 +8546,16 @@
       <c r="L33" s="46"/>
       <c r="M33" s="46"/>
       <c r="N33" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O33" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P33" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q33" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S33" s="53"/>
     </row>
@@ -8445,16 +8570,16 @@
       <c r="L34" s="46"/>
       <c r="M34" s="46"/>
       <c r="N34" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O34" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P34" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q34" s="19" t="s">
         <v>164</v>
-      </c>
-      <c r="Q34" s="19" t="s">
-        <v>165</v>
       </c>
       <c r="S34" s="53"/>
     </row>
@@ -8469,16 +8594,16 @@
       <c r="L35" s="46"/>
       <c r="M35" s="46"/>
       <c r="N35" s="59" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="O35" s="9">
         <v>1</v>
       </c>
       <c r="P35" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q35" s="19" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="S35" s="53"/>
     </row>
@@ -8493,16 +8618,16 @@
       <c r="L36" s="46"/>
       <c r="M36" s="46"/>
       <c r="N36" s="59" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="O36" s="9">
         <v>1</v>
       </c>
       <c r="P36" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q36" s="19" t="s">
         <v>56</v>
-      </c>
-      <c r="Q36" s="19" t="s">
-        <v>57</v>
       </c>
       <c r="S36" s="53"/>
     </row>
@@ -8517,46 +8642,46 @@
       <c r="L37" s="62"/>
       <c r="M37" s="62"/>
       <c r="N37" s="38" t="s">
+        <v>223</v>
+      </c>
+      <c r="O37" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="P37" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q37" s="41" t="s">
         <v>224</v>
-      </c>
-      <c r="O37" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="P37" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q37" s="41" t="s">
-        <v>225</v>
       </c>
       <c r="S37" s="53"/>
     </row>
     <row r="38" spans="2:19" ht="15.75" customHeight="1">
       <c r="B38" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C38" s="18" t="s">
+        <v>227</v>
+      </c>
+      <c r="D38" s="14" t="s">
         <v>228</v>
       </c>
-      <c r="D38" s="14" t="s">
-        <v>229</v>
-      </c>
       <c r="E38" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F38" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="G38" s="9" t="s">
         <v>82</v>
-      </c>
-      <c r="G38" s="9" t="s">
-        <v>83</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="27"/>
       <c r="J38" s="27"/>
-      <c r="K38" s="98" t="s">
-        <v>106</v>
-      </c>
-      <c r="L38" s="81"/>
-      <c r="M38" s="99"/>
+      <c r="K38" s="100" t="s">
+        <v>105</v>
+      </c>
+      <c r="L38" s="84"/>
+      <c r="M38" s="101"/>
       <c r="N38" s="24"/>
       <c r="Q38" s="25"/>
       <c r="S38" s="51"/>
@@ -8566,13 +8691,13 @@
       <c r="C39" s="38"/>
       <c r="D39" s="16"/>
       <c r="E39" s="9" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G39" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H39" s="24"/>
       <c r="K39" s="56"/>
@@ -8586,42 +8711,42 @@
     </row>
     <row r="40" spans="2:19" ht="15.75" customHeight="1">
       <c r="B40" s="14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C40" s="19" t="s">
+        <v>235</v>
+      </c>
+      <c r="D40" s="17" t="s">
         <v>236</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>237</v>
       </c>
       <c r="E40" s="18"/>
       <c r="F40" s="20"/>
       <c r="G40" s="20"/>
       <c r="H40" s="18" t="s">
+        <v>237</v>
+      </c>
+      <c r="I40" s="20" t="s">
         <v>238</v>
       </c>
-      <c r="I40" s="20" t="s">
+      <c r="J40" s="20" t="s">
         <v>239</v>
       </c>
-      <c r="J40" s="20" t="s">
-        <v>240</v>
-      </c>
-      <c r="K40" s="91" t="s">
-        <v>106</v>
-      </c>
-      <c r="L40" s="92"/>
-      <c r="M40" s="93"/>
+      <c r="K40" s="102" t="s">
+        <v>105</v>
+      </c>
+      <c r="L40" s="98"/>
+      <c r="M40" s="99"/>
       <c r="N40" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O40" s="20">
         <v>1</v>
       </c>
       <c r="P40" s="20" t="s">
+        <v>81</v>
+      </c>
+      <c r="Q40" s="22" t="s">
         <v>82</v>
-      </c>
-      <c r="Q40" s="22" t="s">
-        <v>83</v>
       </c>
       <c r="S40" s="53"/>
     </row>
@@ -8639,16 +8764,16 @@
       <c r="L41" s="46"/>
       <c r="M41" s="64"/>
       <c r="N41" s="17" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="O41" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P41" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q41" s="19" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="S41" s="53"/>
     </row>
@@ -8666,16 +8791,16 @@
       <c r="L42" s="46"/>
       <c r="M42" s="64"/>
       <c r="N42" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O42" s="9">
         <v>1</v>
       </c>
       <c r="P42" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q42" s="19" t="s">
         <v>108</v>
-      </c>
-      <c r="Q42" s="19" t="s">
-        <v>109</v>
       </c>
       <c r="S42" s="53"/>
     </row>
@@ -8693,16 +8818,16 @@
       <c r="L43" s="46"/>
       <c r="M43" s="64"/>
       <c r="N43" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O43" s="9">
         <v>1</v>
       </c>
       <c r="P43" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="Q43" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="S43" s="53"/>
     </row>
@@ -8720,16 +8845,16 @@
       <c r="L44" s="46"/>
       <c r="M44" s="64"/>
       <c r="N44" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="O44" s="9">
         <v>1</v>
       </c>
       <c r="P44" s="9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="Q44" s="19" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="S44" s="53"/>
     </row>
@@ -8747,16 +8872,16 @@
       <c r="L45" s="46"/>
       <c r="M45" s="64"/>
       <c r="N45" s="17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O45" s="9">
         <v>1</v>
       </c>
       <c r="P45" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q45" s="19" t="s">
         <v>66</v>
-      </c>
-      <c r="Q45" s="19" t="s">
-        <v>67</v>
       </c>
       <c r="S45" s="53"/>
     </row>
@@ -8774,16 +8899,16 @@
       <c r="L46" s="46"/>
       <c r="M46" s="64"/>
       <c r="N46" s="17" t="s">
+        <v>68</v>
+      </c>
+      <c r="O46" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P46" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="O46" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="P46" s="9" t="s">
-        <v>70</v>
-      </c>
       <c r="Q46" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="S46" s="53"/>
     </row>
@@ -8801,16 +8926,16 @@
       <c r="L47" s="46"/>
       <c r="M47" s="64"/>
       <c r="N47" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="O47" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P47" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="O47" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="P47" s="9" t="s">
+      <c r="Q47" s="19" t="s">
         <v>155</v>
-      </c>
-      <c r="Q47" s="19" t="s">
-        <v>156</v>
       </c>
       <c r="S47" s="53"/>
     </row>
@@ -8828,16 +8953,16 @@
       <c r="L48" s="46"/>
       <c r="M48" s="64"/>
       <c r="N48" s="17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O48" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P48" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q48" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="S48" s="50"/>
     </row>
@@ -8855,16 +8980,16 @@
       <c r="L49" s="46"/>
       <c r="M49" s="64"/>
       <c r="N49" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="O49" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="P49" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q49" s="19" t="s">
         <v>164</v>
-      </c>
-      <c r="Q49" s="19" t="s">
-        <v>165</v>
       </c>
       <c r="S49" s="51"/>
     </row>
@@ -8882,16 +9007,16 @@
       <c r="L50" s="46"/>
       <c r="M50" s="64"/>
       <c r="N50" s="59" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O50" s="9">
         <v>1</v>
       </c>
       <c r="P50" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="Q50" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S50" s="53"/>
     </row>
@@ -8909,16 +9034,16 @@
       <c r="L51" s="46"/>
       <c r="M51" s="64"/>
       <c r="N51" s="59" t="s">
+        <v>243</v>
+      </c>
+      <c r="O51" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="P51" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q51" s="19" t="s">
         <v>244</v>
-      </c>
-      <c r="O51" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="P51" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q51" s="19" t="s">
-        <v>245</v>
       </c>
       <c r="S51" s="65"/>
     </row>
@@ -8936,38 +9061,38 @@
       <c r="L52" s="62"/>
       <c r="M52" s="66"/>
       <c r="N52" s="38" t="s">
+        <v>245</v>
+      </c>
+      <c r="O52" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="P52" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q52" s="41" t="s">
         <v>246</v>
-      </c>
-      <c r="O52" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="P52" s="58" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q52" s="41" t="s">
-        <v>247</v>
       </c>
       <c r="S52" s="67"/>
     </row>
     <row r="53" spans="1:19" ht="15.75" customHeight="1">
       <c r="B53" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C53" s="18" t="s">
+        <v>249</v>
+      </c>
+      <c r="D53" s="18" t="s">
         <v>250</v>
-      </c>
-      <c r="D53" s="18" t="s">
-        <v>251</v>
       </c>
       <c r="E53" s="17"/>
       <c r="F53" s="9"/>
       <c r="G53" s="9"/>
       <c r="H53" s="24"/>
-      <c r="K53" s="98" t="s">
-        <v>106</v>
-      </c>
-      <c r="L53" s="81"/>
-      <c r="M53" s="99"/>
+      <c r="K53" s="100" t="s">
+        <v>105</v>
+      </c>
+      <c r="L53" s="84"/>
+      <c r="M53" s="101"/>
       <c r="N53" s="26"/>
       <c r="O53" s="27"/>
       <c r="P53" s="27"/>
@@ -9020,48 +9145,53 @@
     </row>
     <row r="58" spans="1:19" ht="15.75" customHeight="1">
       <c r="K58" s="97" t="s">
-        <v>106</v>
-      </c>
-      <c r="L58" s="92"/>
-      <c r="M58" s="93"/>
+        <v>105</v>
+      </c>
+      <c r="L58" s="98"/>
+      <c r="M58" s="99"/>
       <c r="S58" s="53"/>
     </row>
     <row r="59" spans="1:19" ht="15.75" customHeight="1">
       <c r="K59" s="18" t="s">
+        <v>251</v>
+      </c>
+      <c r="L59" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="M59" s="22" t="s">
         <v>252</v>
-      </c>
-      <c r="L59" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="M59" s="22" t="s">
-        <v>253</v>
       </c>
       <c r="S59" s="51"/>
     </row>
     <row r="60" spans="1:19" ht="15.75" customHeight="1">
       <c r="K60" s="17" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="L60" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M60" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" spans="1:19" ht="15.75" customHeight="1">
       <c r="K61" s="30" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L61" s="40" t="s">
+        <v>39</v>
+      </c>
+      <c r="M61" s="36" t="s">
         <v>40</v>
-      </c>
-      <c r="M61" s="36" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="K9:M9"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="K23:M23"/>
     <mergeCell ref="H1:J1"/>
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="K54:M54"/>
@@ -9072,11 +9202,6 @@
     <mergeCell ref="K15:M15"/>
     <mergeCell ref="K25:M25"/>
     <mergeCell ref="K38:M38"/>
-    <mergeCell ref="N1:Q1"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="K9:M9"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="K23:M23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9101,14 +9226,14 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
       <c r="A1" s="48" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="86" t="s">
-        <v>120</v>
-      </c>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="88"/>
+        <v>19</v>
+      </c>
+      <c r="B1" s="89" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" s="90"/>
+      <c r="D1" s="90"/>
+      <c r="E1" s="91"/>
       <c r="F1" s="49"/>
       <c r="G1" s="49"/>
       <c r="H1" s="49"/>
@@ -9134,626 +9259,626 @@
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="43"/>
       <c r="B2" s="12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C3" s="20">
         <v>1</v>
       </c>
       <c r="D3" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="E3" s="22" t="s">
         <v>125</v>
-      </c>
-      <c r="E3" s="22" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
       <c r="A4" s="24"/>
       <c r="B4" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D4" s="9" t="s">
+      <c r="E4" s="19" t="s">
         <v>128</v>
-      </c>
-      <c r="E4" s="19" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
       <c r="A5" s="24"/>
       <c r="B5" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="19" t="s">
         <v>130</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="19" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
       <c r="A6" s="30"/>
       <c r="B6" s="40" t="s">
+        <v>131</v>
+      </c>
+      <c r="C6" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="C6" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="40" t="s">
+      <c r="E6" s="41" t="s">
         <v>133</v>
-      </c>
-      <c r="E6" s="41" t="s">
-        <v>134</v>
       </c>
       <c r="H6" s="52"/>
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
       <c r="A7" s="18" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C7" s="20">
         <v>1</v>
       </c>
       <c r="D7" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E7" s="22" t="s">
         <v>104</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>105</v>
       </c>
       <c r="H7" s="52"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1">
       <c r="A8" s="24"/>
       <c r="B8" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C8" s="9">
         <v>1</v>
       </c>
       <c r="D8" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="19" t="s">
         <v>111</v>
-      </c>
-      <c r="E8" s="19" t="s">
-        <v>112</v>
       </c>
       <c r="H8" s="52"/>
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
       <c r="A9" s="24"/>
       <c r="B9" s="9" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E9" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H9" s="52"/>
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
       <c r="A10" s="30"/>
       <c r="B10" s="40" t="s">
+        <v>138</v>
+      </c>
+      <c r="C10" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="41" t="s">
         <v>139</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="40" t="s">
-        <v>108</v>
-      </c>
-      <c r="E10" s="41" t="s">
-        <v>140</v>
       </c>
       <c r="H10" s="52"/>
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
       <c r="A11" s="18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B11" s="20" t="s">
+        <v>140</v>
+      </c>
+      <c r="C11" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="20" t="s">
         <v>141</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D11" s="20" t="s">
+      <c r="E11" s="22" t="s">
         <v>142</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
       <c r="A12" s="30"/>
       <c r="B12" s="40" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="C12" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="9" t="s">
+      <c r="E12" s="41" t="s">
         <v>146</v>
-      </c>
-      <c r="E12" s="41" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
       <c r="A13" s="18" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B13" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="C13" s="20" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="22" t="s">
         <v>148</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="22" t="s">
-        <v>149</v>
       </c>
       <c r="F13" s="51"/>
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
       <c r="A14" s="24"/>
       <c r="B14" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="19" t="s">
         <v>150</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D14" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>151</v>
       </c>
       <c r="F14" s="51"/>
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
       <c r="A15" s="30"/>
       <c r="B15" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="C15" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="41" t="s">
         <v>152</v>
-      </c>
-      <c r="C15" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="D15" s="40" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="41" t="s">
-        <v>153</v>
       </c>
       <c r="F15" s="51"/>
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
       <c r="A16" s="32" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="34" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="51"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1">
       <c r="A17" s="32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="E17" s="44" t="s">
         <v>159</v>
-      </c>
-      <c r="E17" s="44" t="s">
-        <v>160</v>
       </c>
       <c r="F17" s="51"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1">
       <c r="A18" s="32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
       <c r="D18" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E18" s="44" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1">
       <c r="A19" s="18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C19" s="20">
         <v>1</v>
       </c>
       <c r="D19" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="E19" s="22" t="s">
         <v>169</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1">
       <c r="A20" s="30"/>
       <c r="B20" s="40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="40">
         <v>1</v>
       </c>
       <c r="D20" s="40" t="s">
+        <v>170</v>
+      </c>
+      <c r="E20" s="41" t="s">
         <v>171</v>
-      </c>
-      <c r="E20" s="41" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1">
       <c r="A21" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="55" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C21" s="20">
         <v>1</v>
       </c>
       <c r="D21" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="E21" s="22" t="s">
         <v>176</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1">
       <c r="A22" s="24"/>
       <c r="B22" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="C22" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="9" t="s">
+      <c r="E22" s="19" t="s">
         <v>179</v>
-      </c>
-      <c r="E22" s="19" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1">
       <c r="A23" s="24"/>
       <c r="B23" s="9" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C23" s="9">
         <v>1</v>
       </c>
       <c r="D23" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="E23" s="19" t="s">
         <v>182</v>
-      </c>
-      <c r="E23" s="19" t="s">
-        <v>183</v>
       </c>
       <c r="F23" s="51"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1">
       <c r="A24" s="24"/>
       <c r="B24" s="9" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C24" s="9">
         <v>1</v>
       </c>
       <c r="D24" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="E24" s="19" t="s">
         <v>185</v>
-      </c>
-      <c r="E24" s="19" t="s">
-        <v>186</v>
       </c>
       <c r="F24" s="51"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1">
       <c r="A25" s="24"/>
       <c r="B25" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="C25" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="47" t="s">
+      <c r="E25" s="19" t="s">
         <v>188</v>
-      </c>
-      <c r="E25" s="19" t="s">
-        <v>189</v>
       </c>
       <c r="F25" s="51"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1">
       <c r="A26" s="30"/>
       <c r="B26" s="40" t="s">
+        <v>189</v>
+      </c>
+      <c r="C26" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="D26" s="40" t="s">
         <v>190</v>
       </c>
-      <c r="C26" s="40" t="s">
-        <v>43</v>
-      </c>
-      <c r="D26" s="40" t="s">
+      <c r="E26" s="41" t="s">
         <v>191</v>
-      </c>
-      <c r="E26" s="41" t="s">
-        <v>192</v>
       </c>
       <c r="F26" s="51"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1">
       <c r="A27" s="32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
       <c r="D27" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E27" s="44" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F27" s="51"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1">
       <c r="A28" s="57" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E28" s="44" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F28" s="52"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1">
       <c r="A29" s="32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="34" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="E29" s="44"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1">
       <c r="A30" s="32" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
       <c r="D30" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E30" s="44" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1">
       <c r="A31" s="32" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E31" s="44" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1">
       <c r="A32" s="18" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B32" s="55" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C32" s="20">
         <v>1</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E32" s="22" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1">
       <c r="A33" s="30"/>
       <c r="B33" s="58" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C33" s="40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D33" s="40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E33" s="41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1">
       <c r="A34" s="32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="E34" s="44" t="s">
         <v>205</v>
-      </c>
-      <c r="E34" s="44" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1">
       <c r="A35" s="32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
       <c r="D35" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="E35" s="44" t="s">
         <v>207</v>
-      </c>
-      <c r="E35" s="44" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1">
       <c r="A36" s="60" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B36" s="20" t="s">
+        <v>215</v>
+      </c>
+      <c r="C36" s="20" t="s">
         <v>216</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="D36" s="20" t="s">
         <v>217</v>
       </c>
-      <c r="D36" s="20" t="s">
+      <c r="E36" s="22" t="s">
         <v>218</v>
-      </c>
-      <c r="E36" s="22" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1">
       <c r="A37" s="18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B37" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C37" s="20">
         <v>1</v>
       </c>
       <c r="D37" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E37" s="22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1">
       <c r="A38" s="30"/>
       <c r="B38" s="40" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C38" s="40">
         <v>1</v>
       </c>
       <c r="D38" s="40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E38" s="41" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1">
       <c r="A39" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B39" s="27"/>
       <c r="C39" s="27"/>
       <c r="D39" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="E39" s="22" t="s">
         <v>226</v>
-      </c>
-      <c r="E39" s="22" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1">
       <c r="A40" s="60" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B40" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C40" s="20">
         <v>1</v>
       </c>
       <c r="D40" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="E40" s="22" t="s">
         <v>231</v>
-      </c>
-      <c r="E40" s="22" t="s">
-        <v>232</v>
       </c>
       <c r="G40" s="50"/>
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1">
       <c r="A41" s="24"/>
       <c r="B41" s="9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C41" s="9">
         <v>1</v>
       </c>
       <c r="D41" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="E41" s="19" t="s">
         <v>234</v>
-      </c>
-      <c r="E41" s="19" t="s">
-        <v>235</v>
       </c>
       <c r="G41" s="51"/>
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1">
       <c r="A42" s="32" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="34" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E42" s="44" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G42" s="54"/>
     </row>

</xml_diff>

<commit_message>
Updates for new environment
</commit_message>
<xml_diff>
--- a/Mifos-io-environment-details.xlsx
+++ b/Mifos-io-environment-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sconrad/DIAL/mifos/mifos-io-configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405081F4-8165-194B-B747-D83B3A1AA597}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4FBA650-3B6B-1F47-BAD8-8B519DD2BD60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1220" yWindow="840" windowWidth="27860" windowHeight="17580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="314">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="315">
   <si>
     <t>URL</t>
   </si>
@@ -991,6 +991,9 @@
   </si>
   <si>
     <t>http://fineract3.mifos.io:9002/?baseApiUrl=https://fineract3.mifos.io:8443&amp;tenantIdentifier=tn06</t>
+  </si>
+  <si>
+    <t>http://paymenthub3.mifos.io/channel</t>
   </si>
 </sst>
 </file>
@@ -1794,10 +1797,10 @@
   <dimension ref="A1:Y1011"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G10" sqref="G10"/>
+      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -2350,10 +2353,10 @@
         <v>271</v>
       </c>
       <c r="F25" s="82" t="s">
-        <v>271</v>
-      </c>
-      <c r="G25" s="13" t="s">
-        <v>271</v>
+        <v>314</v>
+      </c>
+      <c r="G25" s="82" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="26" spans="1:25" ht="15.75" customHeight="1">
@@ -6515,6 +6518,7 @@
     <hyperlink ref="F25" r:id="rId35" xr:uid="{E3F7CD8E-6CC9-DB49-AF54-B1C5250E5C19}"/>
     <hyperlink ref="F28" r:id="rId36" xr:uid="{D015083F-7166-964B-891A-362371B8E696}"/>
     <hyperlink ref="G28" r:id="rId37" xr:uid="{10B28FE3-1296-5B4C-ACBA-40A3F51BA3A3}"/>
+    <hyperlink ref="G25" r:id="rId38" xr:uid="{EBC51B82-9E4B-1843-B27A-746F2761A73B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updates to environment document
</commit_message>
<xml_diff>
--- a/Mifos-io-environment-details.xlsx
+++ b/Mifos-io-environment-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sconrad/DIAL/mifos/mifos-io-configuration/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4FBA650-3B6B-1F47-BAD8-8B519DD2BD60}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D36FDCF-A633-574F-A541-C44AFE2B0C3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1220" yWindow="840" windowWidth="27860" windowHeight="17580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1797,10 +1797,10 @@
   <dimension ref="A1:Y1011"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G23" sqref="G23"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>

</xml_diff>